<commit_message>
#234 Updated with BT detector at Highpark
Green ones are high priority. Green DU_UN and BD_AV is along the Active TO bike lane. May be of interest. Dufferin (both direction) is a low priority.

Routes along Roncesvalles is red as BD_DU is not working. But might be a route of interest in future.

Highpark-Runnymede both directions and Highpark-Dufferin both directions are the four added routes of immediate interest.
</commit_message>
<xml_diff>
--- a/bluetooth/update/Bliptrack TT Routes - 2020-09-08.xlsx
+++ b/bluetooth/update/Bliptrack TT Routes - 2020-09-08.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mohan\Documents\GitHub\Mohan_BT_detector_review\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mohan\Documents\GitHub\bdit_data-sources\bluetooth\update\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F8C90A9-C258-4ADC-BCC5-799A74CFC7D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A24DBF-69C2-46F7-B89A-6B6B790F302F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Reports" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Locations!$A$3:$F$62</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Reports!$A$2:$AF$146</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Reports!$A$2:$AF$142</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -98,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1335" uniqueCount="696">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1295" uniqueCount="692">
   <si>
     <t>Start point</t>
   </si>
@@ -1645,24 +1645,12 @@
     <t>5263_1, 5263_2, 5268_1, 5268_2</t>
   </si>
   <si>
-    <t>BD_DU+BL_RU</t>
-  </si>
-  <si>
     <t>BL_RU</t>
   </si>
   <si>
-    <t>5268_1, 5268_2, 9312_1, 9312_2</t>
-  </si>
-  <si>
-    <t>BL_RU+BD_DU</t>
-  </si>
-  <si>
     <t>9312_1, 9312_2</t>
   </si>
   <si>
-    <t>9312_1, 9312_2, 5268_1, 5268_2</t>
-  </si>
-  <si>
     <t>Dufferin NB</t>
   </si>
   <si>
@@ -1699,12 +1687,6 @@
     <t>DT3_Dufferin-SB_Bloor-to-College</t>
   </si>
   <si>
-    <t>DT3_Bloor-WB_Dundas-to-Runnymede</t>
-  </si>
-  <si>
-    <t>DT3_Bloor-EB_Runnymede-to-Dundas</t>
-  </si>
-  <si>
     <t>DT3_College-EB_Dufferin-to-Ossington</t>
   </si>
   <si>
@@ -2050,54 +2032,9 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>BL_RU pull data false. No datetime_bin data populated</t>
-  </si>
-  <si>
     <t>new bikelanes</t>
   </si>
   <si>
-    <t>DT3_Bloor-EB_Dundas-to-Dufferin</t>
-  </si>
-  <si>
-    <t>DT3_Bloor-EB_Dufferin-to-Ossington</t>
-  </si>
-  <si>
-    <t>DT3_Bloor-WB_Dufferin-to-Dundas</t>
-  </si>
-  <si>
-    <t>DT3_Bloor-WB_Ossington-to-Dufferin</t>
-  </si>
-  <si>
-    <t>BD_OS pulling data is true but no datetime_bin data populated in aggr_5min table</t>
-  </si>
-  <si>
-    <t>BD_DF no data pulled in aggr_5min table. CO_DF no data pulled record exist.  DU_DF last pulled data was on 2020 Feb 07. QU_DF last data pulled was 2018/10/10 is inactive and only KN_DF is active and sending signals.</t>
-  </si>
-  <si>
-    <t>DT3_Dufferin-NB_King-to-Bloor</t>
-  </si>
-  <si>
-    <t>KN_DF</t>
-  </si>
-  <si>
-    <t>KN_DF+BD_DF</t>
-  </si>
-  <si>
-    <t>9002_1, 9002_2</t>
-  </si>
-  <si>
-    <t>9002_1, 9002_2, 9096_1, 9096_2</t>
-  </si>
-  <si>
-    <t>DT3_Dufferin-SB_Bloor-to-King</t>
-  </si>
-  <si>
-    <t>BD_DF+KN_DF</t>
-  </si>
-  <si>
-    <t>9096_1, 9096_2, 9002_1, 9002_2</t>
-  </si>
-  <si>
     <t>DT3_Roncesvalles-NB_Queen-to-Bloor</t>
   </si>
   <si>
@@ -2119,39 +2056,12 @@
     <t>5268_1, 5268_2, 9021_1, 9021_2</t>
   </si>
   <si>
-    <t>QU_RO is active. Sending data as of 2020-09-16</t>
-  </si>
-  <si>
-    <t>BD_DU pull data is true but no data on aggr_5min table</t>
-  </si>
-  <si>
-    <t>5266_1, 5266_2, 9098_1, 9098_2</t>
-  </si>
-  <si>
-    <t>DT3_Ossington-SB_Bloor-to-Dundas</t>
-  </si>
-  <si>
-    <t>DT3_Ossington-NB_Dundas-to-Bloor</t>
-  </si>
-  <si>
-    <t>BD_OS+DU_OS</t>
-  </si>
-  <si>
-    <t>DU_OS+BD_OS</t>
-  </si>
-  <si>
-    <t>9098_1, 9098_2, 5266_1, 5266_2</t>
-  </si>
-  <si>
     <t>bike lane high priority</t>
   </si>
   <si>
     <t>bike lane low priority</t>
   </si>
   <si>
-    <t>BD_DF pulling data is true but no datetime_bin data populated in aggr_5 min table</t>
-  </si>
-  <si>
     <t>DT3_University-NB_Dundas-to-Bloor</t>
   </si>
   <si>
@@ -2185,7 +2095,85 @@
     <t>DU_UN reporting data until 2020-09-16, ActiveTO bike lane</t>
   </si>
   <si>
-    <t>DU_OS no data pulled at all</t>
+    <t>BD_HP</t>
+  </si>
+  <si>
+    <t>BL_RU+BD_HP</t>
+  </si>
+  <si>
+    <t>9312_1, 9312_2, 5819_1, 5819_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5819_1, 5819_2</t>
+  </si>
+  <si>
+    <t>DT3_Bloor-EB_Runnymede-to-Highpark</t>
+  </si>
+  <si>
+    <t>DT3_Bloor-WB_Highpark-to-Runnymede</t>
+  </si>
+  <si>
+    <t>BD_HP+BL_RU</t>
+  </si>
+  <si>
+    <t>5819_1, 5819_2, 9312_1, 9312_2</t>
+  </si>
+  <si>
+    <t>DT3_Bloor-EB_Highpark-to-Dufferin</t>
+  </si>
+  <si>
+    <t>BD_HP+BD_DF</t>
+  </si>
+  <si>
+    <t>5819_1, 5819_2, 9096_1, 9096_2</t>
+  </si>
+  <si>
+    <t>BD_DF+BD_HP</t>
+  </si>
+  <si>
+    <t>9096_1, 9096_2, 5819_1, 5819_2</t>
+  </si>
+  <si>
+    <t>5819_1, 5819_2</t>
+  </si>
+  <si>
+    <t>DT3_Bloor-WB_Dufferin-to-Highpark</t>
+  </si>
+  <si>
+    <t>BD_HP active in JJ table. New detector</t>
+  </si>
+  <si>
+    <t>BD_DF active in JJ table but no datetime_bin data populated in aggr_5 min table</t>
+  </si>
+  <si>
+    <t>DT3_Dufferin-NB_Dundas-to-Bloor</t>
+  </si>
+  <si>
+    <t>DT3_Dufferin-SB_Bloor-to-Dundas</t>
+  </si>
+  <si>
+    <t>BD_DF+DU_DF</t>
+  </si>
+  <si>
+    <t>DU_DF+BD_DF</t>
+  </si>
+  <si>
+    <t>9039_1, 9039_2, 9096_1, 9096_2</t>
+  </si>
+  <si>
+    <t>9096_1, 9096_2, 9039_1, 9039_2</t>
+  </si>
+  <si>
+    <t>BL_RU active in JJ table but no datetime_bin data populated in aggr_5min table</t>
+  </si>
+  <si>
+    <t>QU_RO is active. Sending data as of 2020-09-16. But BD_DU is not in JJ list of active detectors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BD_DU is not in JJ list of active detectors. </t>
+  </si>
+  <si>
+    <t>DU_DF active in JJ table  but last data received in aggr_5 min table was on 2020-02-07</t>
   </si>
 </sst>
 </file>
@@ -2285,7 +2273,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2342,6 +2330,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2499,7 +2493,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2567,7 +2561,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2881,33 +2883,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AG156"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:AG149"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="AB121" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AG154" sqref="AG154"/>
+      <pane xSplit="5" ySplit="99" topLeftCell="AF100" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A100" sqref="A100"/>
+      <selection pane="bottomRight" activeCell="A140" sqref="A140:XFD141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22" style="1" customWidth="1"/>
-    <col min="2" max="2" width="36.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" style="1" customWidth="1"/>
     <col min="5" max="5" width="1.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="7.42578125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="4.140625" style="5" customWidth="1"/>
     <col min="7" max="7" width="14.7109375" style="1" customWidth="1"/>
     <col min="8" max="8" width="15.7109375" style="1" customWidth="1"/>
     <col min="9" max="9" width="25.42578125" style="1" customWidth="1"/>
     <col min="10" max="10" width="9" style="1" customWidth="1"/>
     <col min="11" max="12" width="15.7109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="10.5703125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="7.85546875" style="1" customWidth="1"/>
     <col min="14" max="14" width="2.85546875" style="1" customWidth="1"/>
-    <col min="15" max="15" width="13" style="5" customWidth="1"/>
+    <col min="15" max="15" width="5.85546875" style="5" customWidth="1"/>
     <col min="16" max="16" width="13.5703125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7" style="1" customWidth="1"/>
     <col min="18" max="19" width="15.7109375" style="1" customWidth="1"/>
     <col min="20" max="20" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
@@ -2925,53 +2928,53 @@
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>651</v>
-      </c>
-      <c r="B1" s="52" t="s">
+        <v>644</v>
+      </c>
+      <c r="B1" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="52"/>
-      <c r="D1" s="53" t="s">
+      <c r="C1" s="56"/>
+      <c r="D1" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="54" t="s">
+      <c r="E1" s="57"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="56" t="s">
+      <c r="N1" s="58"/>
+      <c r="O1" s="58"/>
+      <c r="P1" s="58"/>
+      <c r="Q1" s="58"/>
+      <c r="R1" s="58"/>
+      <c r="S1" s="58"/>
+      <c r="T1" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="U1" s="56"/>
-      <c r="V1" s="56"/>
-      <c r="W1" s="57" t="s">
+      <c r="U1" s="60"/>
+      <c r="V1" s="60"/>
+      <c r="W1" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="X1" s="57"/>
-      <c r="Y1" s="57"/>
-      <c r="Z1" s="55" t="s">
+      <c r="X1" s="61"/>
+      <c r="Y1" s="61"/>
+      <c r="Z1" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="AA1" s="55"/>
-      <c r="AB1" s="55"/>
-      <c r="AC1" s="55"/>
-      <c r="AD1" s="55"/>
-      <c r="AE1" s="55"/>
-      <c r="AF1" s="55"/>
+      <c r="AA1" s="59"/>
+      <c r="AB1" s="59"/>
+      <c r="AC1" s="59"/>
+      <c r="AD1" s="59"/>
+      <c r="AE1" s="59"/>
+      <c r="AF1" s="59"/>
       <c r="AG1" s="1" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.2">
@@ -3069,7 +3072,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="B3" s="19" t="s">
         <v>145</v>
       </c>
@@ -3119,7 +3122,7 @@
         <v>-79.435443899999996</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="B4" s="19" t="s">
         <v>151</v>
       </c>
@@ -3169,7 +3172,7 @@
         <v>-79.425572900000006</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="B5" s="19" t="s">
         <v>155</v>
       </c>
@@ -3219,7 +3222,7 @@
         <v>-79.411196700000005</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="B6" s="19" t="s">
         <v>159</v>
       </c>
@@ -3269,7 +3272,7 @@
         <v>-79.403815300000005</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="B7" s="19" t="s">
         <v>163</v>
       </c>
@@ -3319,7 +3322,7 @@
         <v>-79.394137900000004</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="B8" s="19" t="s">
         <v>167</v>
       </c>
@@ -3369,7 +3372,7 @@
         <v>-79.386713499999999</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="B9" s="19" t="s">
         <v>171</v>
       </c>
@@ -3419,7 +3422,7 @@
         <v>-79.380565899999993</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="B10" s="19" t="s">
         <v>175</v>
       </c>
@@ -3469,7 +3472,7 @@
         <v>-79.371070900000007</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="B11" s="19" t="s">
         <v>179</v>
       </c>
@@ -3519,7 +3522,7 @@
         <v>-79.358453800000007</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="B12" s="19" t="s">
         <v>183</v>
       </c>
@@ -3569,7 +3572,7 @@
         <v>-79.332368000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="B13" s="19" t="s">
         <v>188</v>
       </c>
@@ -3619,7 +3622,7 @@
         <v>-79.312768000000005</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="B14" s="19" t="s">
         <v>192</v>
       </c>
@@ -3669,7 +3672,7 @@
         <v>-79.351301000000007</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="B15" s="19" t="s">
         <v>198</v>
       </c>
@@ -3719,7 +3722,7 @@
         <v>-79.334245999999993</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="B16" s="19" t="s">
         <v>202</v>
       </c>
@@ -3769,7 +3772,7 @@
         <v>-79.317549999999997</v>
       </c>
     </row>
-    <row r="17" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B17" s="19" t="s">
         <v>206</v>
       </c>
@@ -3819,7 +3822,7 @@
         <v>-79.348656000000005</v>
       </c>
     </row>
-    <row r="18" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B18" s="19" t="s">
         <v>212</v>
       </c>
@@ -3869,7 +3872,7 @@
         <v>-79.329459999999997</v>
       </c>
     </row>
-    <row r="19" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B19" s="19" t="s">
         <v>217</v>
       </c>
@@ -3919,7 +3922,7 @@
         <v>-79.316207000000006</v>
       </c>
     </row>
-    <row r="20" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B20" s="19" t="s">
         <v>221</v>
       </c>
@@ -3969,7 +3972,7 @@
         <v>-79.307919999999996</v>
       </c>
     </row>
-    <row r="21" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B21" s="19" t="s">
         <v>226</v>
       </c>
@@ -4019,7 +4022,7 @@
         <v>-79.382057200000006</v>
       </c>
     </row>
-    <row r="22" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B22" s="19" t="s">
         <v>232</v>
       </c>
@@ -4069,7 +4072,7 @@
         <v>-79.375823800000006</v>
       </c>
     </row>
-    <row r="23" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B23" s="19" t="s">
         <v>236</v>
       </c>
@@ -4119,7 +4122,7 @@
         <v>-79.367079700000005</v>
       </c>
     </row>
-    <row r="24" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B24" s="19" t="s">
         <v>240</v>
       </c>
@@ -4169,7 +4172,7 @@
         <v>-79.352745900000002</v>
       </c>
     </row>
-    <row r="25" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B25" s="19" t="s">
         <v>244</v>
       </c>
@@ -4219,7 +4222,7 @@
         <v>-79.328001999999998</v>
       </c>
     </row>
-    <row r="26" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B26" s="19" t="s">
         <v>248</v>
       </c>
@@ -4269,7 +4272,7 @@
         <v>-79.347048000000001</v>
       </c>
     </row>
-    <row r="27" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B27" s="19" t="s">
         <v>254</v>
       </c>
@@ -4319,7 +4322,7 @@
         <v>-79.328438000000006</v>
       </c>
     </row>
-    <row r="28" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B28" s="19" t="s">
         <v>258</v>
       </c>
@@ -4369,7 +4372,7 @@
         <v>-79.314841000000001</v>
       </c>
     </row>
-    <row r="29" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B29" s="19" t="s">
         <v>262</v>
       </c>
@@ -4419,7 +4422,7 @@
         <v>-79.305773000000002</v>
       </c>
     </row>
-    <row r="30" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B30" s="19" t="s">
         <v>267</v>
       </c>
@@ -4469,7 +4472,7 @@
         <v>-79.325288999999998</v>
       </c>
     </row>
-    <row r="31" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B31" s="19" t="s">
         <v>273</v>
       </c>
@@ -4519,7 +4522,7 @@
         <v>-79.305773000000002</v>
       </c>
     </row>
-    <row r="32" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B32" s="19" t="s">
         <v>276</v>
       </c>
@@ -4569,7 +4572,7 @@
         <v>-79.332368000000002</v>
       </c>
     </row>
-    <row r="33" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B33" s="19" t="s">
         <v>280</v>
       </c>
@@ -4619,7 +4622,7 @@
         <v>-79.358453800000007</v>
       </c>
     </row>
-    <row r="34" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B34" s="19" t="s">
         <v>283</v>
       </c>
@@ -4669,7 +4672,7 @@
         <v>-79.371070900000007</v>
       </c>
     </row>
-    <row r="35" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B35" s="19" t="s">
         <v>286</v>
       </c>
@@ -4719,7 +4722,7 @@
         <v>-79.380565899999993</v>
       </c>
     </row>
-    <row r="36" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B36" s="19" t="s">
         <v>290</v>
       </c>
@@ -4769,7 +4772,7 @@
         <v>-79.386713499999999</v>
       </c>
     </row>
-    <row r="37" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B37" s="19" t="s">
         <v>293</v>
       </c>
@@ -4819,7 +4822,7 @@
         <v>-79.394137900000004</v>
       </c>
     </row>
-    <row r="38" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B38" s="19" t="s">
         <v>296</v>
       </c>
@@ -4869,7 +4872,7 @@
         <v>-79.403815300000005</v>
       </c>
     </row>
-    <row r="39" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B39" s="19" t="s">
         <v>299</v>
       </c>
@@ -4919,7 +4922,7 @@
         <v>-79.411196700000005</v>
       </c>
     </row>
-    <row r="40" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B40" s="19" t="s">
         <v>302</v>
       </c>
@@ -4969,7 +4972,7 @@
         <v>-79.425572900000006</v>
       </c>
     </row>
-    <row r="41" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B41" s="19" t="s">
         <v>305</v>
       </c>
@@ -5019,7 +5022,7 @@
         <v>-79.435443899999996</v>
       </c>
     </row>
-    <row r="42" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B42" s="19" t="s">
         <v>308</v>
       </c>
@@ -5069,7 +5072,7 @@
         <v>-79.452438400000005</v>
       </c>
     </row>
-    <row r="43" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B43" s="19" t="s">
         <v>311</v>
       </c>
@@ -5119,7 +5122,7 @@
         <v>-79.317549999999997</v>
       </c>
     </row>
-    <row r="44" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B44" s="19" t="s">
         <v>315</v>
       </c>
@@ -5169,7 +5172,7 @@
         <v>-79.334245999999993</v>
       </c>
     </row>
-    <row r="45" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B45" s="19" t="s">
         <v>319</v>
       </c>
@@ -5219,7 +5222,7 @@
         <v>-79.351301000000007</v>
       </c>
     </row>
-    <row r="46" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B46" s="19" t="s">
         <v>322</v>
       </c>
@@ -5269,7 +5272,7 @@
         <v>-79.366140000000001</v>
       </c>
     </row>
-    <row r="47" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B47" s="19" t="s">
         <v>325</v>
       </c>
@@ -5319,7 +5322,7 @@
         <v>-79.316207000000006</v>
       </c>
     </row>
-    <row r="48" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B48" s="19" t="s">
         <v>329</v>
       </c>
@@ -5369,7 +5372,7 @@
         <v>-79.329459999999997</v>
       </c>
     </row>
-    <row r="49" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B49" s="19" t="s">
         <v>333</v>
       </c>
@@ -5419,7 +5422,7 @@
         <v>-79.348656000000005</v>
       </c>
     </row>
-    <row r="50" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B50" s="19" t="s">
         <v>336</v>
       </c>
@@ -5469,7 +5472,7 @@
         <v>-79.352745900000002</v>
       </c>
     </row>
-    <row r="51" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B51" s="19" t="s">
         <v>340</v>
       </c>
@@ -5519,7 +5522,7 @@
         <v>-79.367079700000005</v>
       </c>
     </row>
-    <row r="52" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B52" s="19" t="s">
         <v>343</v>
       </c>
@@ -5569,7 +5572,7 @@
         <v>-79.375823800000006</v>
       </c>
     </row>
-    <row r="53" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B53" s="19" t="s">
         <v>346</v>
       </c>
@@ -5619,7 +5622,7 @@
         <v>-79.382057200000006</v>
       </c>
     </row>
-    <row r="54" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B54" s="19" t="s">
         <v>349</v>
       </c>
@@ -5669,7 +5672,7 @@
         <v>-79.389867800000005</v>
       </c>
     </row>
-    <row r="55" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="55" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B55" s="19" t="s">
         <v>352</v>
       </c>
@@ -5719,7 +5722,7 @@
         <v>-79.314841000000001</v>
       </c>
     </row>
-    <row r="56" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="56" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B56" s="19" t="s">
         <v>356</v>
       </c>
@@ -5769,7 +5772,7 @@
         <v>-79.328438000000006</v>
       </c>
     </row>
-    <row r="57" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B57" s="19" t="s">
         <v>360</v>
       </c>
@@ -5819,7 +5822,7 @@
         <v>-79.347048000000001</v>
       </c>
     </row>
-    <row r="58" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B58" s="19" t="s">
         <v>363</v>
       </c>
@@ -5869,7 +5872,7 @@
         <v>-79.359463888888897</v>
       </c>
     </row>
-    <row r="59" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="59" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B59" s="19" t="s">
         <v>366</v>
       </c>
@@ -5919,7 +5922,7 @@
         <v>-79.325288999999998</v>
       </c>
     </row>
-    <row r="60" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B60" s="19" t="s">
         <v>370</v>
       </c>
@@ -5969,7 +5972,7 @@
         <v>-79.349695999999994</v>
       </c>
     </row>
-    <row r="61" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B61" s="19" t="s">
         <v>373</v>
       </c>
@@ -6019,7 +6022,7 @@
         <v>-79.351301000000007</v>
       </c>
     </row>
-    <row r="62" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B62" s="19" t="s">
         <v>377</v>
       </c>
@@ -6069,7 +6072,7 @@
         <v>-79.352745900000002</v>
       </c>
     </row>
-    <row r="63" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B63" s="19" t="s">
         <v>380</v>
       </c>
@@ -6119,7 +6122,7 @@
         <v>-79.358453800000007</v>
       </c>
     </row>
-    <row r="64" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B64" s="19" t="s">
         <v>383</v>
       </c>
@@ -6169,7 +6172,7 @@
         <v>-79.316207000000006</v>
       </c>
     </row>
-    <row r="65" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B65" s="19" t="s">
         <v>387</v>
       </c>
@@ -6219,7 +6222,7 @@
         <v>-79.317549999999997</v>
       </c>
     </row>
-    <row r="66" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B66" s="19" t="s">
         <v>390</v>
       </c>
@@ -6269,7 +6272,7 @@
         <v>-79.328001999999998</v>
       </c>
     </row>
-    <row r="67" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B67" s="19" t="s">
         <v>394</v>
       </c>
@@ -6319,7 +6322,7 @@
         <v>-79.332368000000002</v>
       </c>
     </row>
-    <row r="68" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B68" s="19" t="s">
         <v>397</v>
       </c>
@@ -6369,7 +6372,7 @@
         <v>-79.375823800000006</v>
       </c>
     </row>
-    <row r="69" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B69" s="19" t="s">
         <v>402</v>
       </c>
@@ -6419,7 +6422,7 @@
         <v>-79.378280599999997</v>
       </c>
     </row>
-    <row r="70" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B70" s="19" t="s">
         <v>406</v>
       </c>
@@ -6469,7 +6472,7 @@
         <v>-79.380565899999993</v>
       </c>
     </row>
-    <row r="71" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B71" s="19" t="s">
         <v>409</v>
       </c>
@@ -6519,7 +6522,7 @@
         <v>-79.329459999999997</v>
       </c>
     </row>
-    <row r="72" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B72" s="19" t="s">
         <v>413</v>
       </c>
@@ -6569,7 +6572,7 @@
         <v>-79.368150999999997</v>
       </c>
     </row>
-    <row r="73" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B73" s="19" t="s">
         <v>418</v>
       </c>
@@ -6619,7 +6622,7 @@
         <v>-79.369504500000005</v>
       </c>
     </row>
-    <row r="74" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B74" s="19" t="s">
         <v>422</v>
       </c>
@@ -6669,7 +6672,7 @@
         <v>-79.371070900000007</v>
       </c>
     </row>
-    <row r="75" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B75" s="19" t="s">
         <v>425</v>
       </c>
@@ -6719,7 +6722,7 @@
         <v>-79.307919999999996</v>
       </c>
     </row>
-    <row r="76" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B76" s="19" t="s">
         <v>429</v>
       </c>
@@ -6769,7 +6772,7 @@
         <v>-79.312768000000005</v>
       </c>
     </row>
-    <row r="77" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B77" s="19" t="s">
         <v>432</v>
       </c>
@@ -6819,7 +6822,7 @@
         <v>-79.382057200000006</v>
       </c>
     </row>
-    <row r="78" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B78" s="19" t="s">
         <v>437</v>
       </c>
@@ -6869,7 +6872,7 @@
         <v>-79.3845034</v>
       </c>
     </row>
-    <row r="79" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B79" s="19" t="s">
         <v>441</v>
       </c>
@@ -6919,7 +6922,7 @@
         <v>-79.386713499999999</v>
       </c>
     </row>
-    <row r="80" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B80" s="19" t="s">
         <v>444</v>
       </c>
@@ -6969,7 +6972,7 @@
         <v>-79.352745900000002</v>
       </c>
     </row>
-    <row r="81" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B81" s="19" t="s">
         <v>448</v>
       </c>
@@ -7019,7 +7022,7 @@
         <v>-79.351301000000007</v>
       </c>
     </row>
-    <row r="82" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B82" s="19" t="s">
         <v>451</v>
       </c>
@@ -7069,7 +7072,7 @@
         <v>-79.348656000000005</v>
       </c>
     </row>
-    <row r="83" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B83" s="19" t="s">
         <v>454</v>
       </c>
@@ -7119,7 +7122,7 @@
         <v>-79.316207000000006</v>
       </c>
     </row>
-    <row r="84" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B84" s="19" t="s">
         <v>458</v>
       </c>
@@ -7169,7 +7172,7 @@
         <v>-79.314841000000001</v>
       </c>
     </row>
-    <row r="85" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B85" s="19" t="s">
         <v>461</v>
       </c>
@@ -7219,7 +7222,7 @@
         <v>-79.328001999999998</v>
       </c>
     </row>
-    <row r="86" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B86" s="19" t="s">
         <v>465</v>
       </c>
@@ -7269,7 +7272,7 @@
         <v>-79.325288999999998</v>
       </c>
     </row>
-    <row r="87" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B87" s="19" t="s">
         <v>468</v>
       </c>
@@ -7319,7 +7322,7 @@
         <v>-79.378280599999997</v>
       </c>
     </row>
-    <row r="88" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B88" s="19" t="s">
         <v>472</v>
       </c>
@@ -7369,7 +7372,7 @@
         <v>-79.375823800000006</v>
       </c>
     </row>
-    <row r="89" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B89" s="19" t="s">
         <v>475</v>
       </c>
@@ -7419,7 +7422,7 @@
         <v>-79.374610000000004</v>
       </c>
     </row>
-    <row r="90" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B90" s="19" t="s">
         <v>478</v>
       </c>
@@ -7469,7 +7472,7 @@
         <v>-79.328438000000006</v>
       </c>
     </row>
-    <row r="91" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B91" s="19" t="s">
         <v>482</v>
       </c>
@@ -7519,7 +7522,7 @@
         <v>-79.369504500000005</v>
       </c>
     </row>
-    <row r="92" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B92" s="19" t="s">
         <v>486</v>
       </c>
@@ -7569,7 +7572,7 @@
         <v>-79.366140000000001</v>
       </c>
     </row>
-    <row r="93" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B93" s="19" t="s">
         <v>489</v>
       </c>
@@ -7619,7 +7622,7 @@
         <v>-79.368150999999997</v>
       </c>
     </row>
-    <row r="94" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B94" s="19" t="s">
         <v>492</v>
       </c>
@@ -7669,7 +7672,7 @@
         <v>-79.307919999999996</v>
       </c>
     </row>
-    <row r="95" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B95" s="19" t="s">
         <v>496</v>
       </c>
@@ -7719,7 +7722,7 @@
         <v>-79.305773000000002</v>
       </c>
     </row>
-    <row r="96" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B96" s="19" t="s">
         <v>499</v>
       </c>
@@ -7769,7 +7772,7 @@
         <v>-79.3845034</v>
       </c>
     </row>
-    <row r="97" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="B97" s="19" t="s">
         <v>503</v>
       </c>
@@ -7819,7 +7822,7 @@
         <v>-79.382057200000006</v>
       </c>
     </row>
-    <row r="98" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="B98" s="19" t="s">
         <v>506</v>
       </c>
@@ -7869,7 +7872,7 @@
         <v>-79.381360000000001</v>
       </c>
     </row>
-    <row r="99" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="B99" s="19" t="s">
         <v>509</v>
       </c>
@@ -7919,124 +7922,124 @@
         <v>-79.452438400000005</v>
       </c>
     </row>
-    <row r="100" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A100" s="47" t="s">
-        <v>681</v>
-      </c>
-      <c r="B100" s="19" t="s">
-        <v>533</v>
-      </c>
-      <c r="C100" s="20" t="s">
+    <row r="100" spans="1:33" s="51" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="51" t="s">
+        <v>652</v>
+      </c>
+      <c r="B100" s="52" t="s">
+        <v>670</v>
+      </c>
+      <c r="C100" s="53" t="s">
         <v>287</v>
       </c>
-      <c r="D100" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="F100" s="1">
-        <v>5268</v>
-      </c>
-      <c r="G100" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="H100" s="1" t="s">
+      <c r="D100" s="51" t="s">
+        <v>665</v>
+      </c>
+      <c r="F100" s="51">
+        <v>5819</v>
+      </c>
+      <c r="G100" s="51" t="s">
+        <v>668</v>
+      </c>
+      <c r="H100" s="51" t="s">
+        <v>671</v>
+      </c>
+      <c r="I100" s="51" t="s">
+        <v>672</v>
+      </c>
+      <c r="J100" s="51">
+        <v>300</v>
+      </c>
+      <c r="K100" s="51">
+        <v>43.653686999999998</v>
+      </c>
+      <c r="L100" s="51">
+        <v>-79.465096000000003</v>
+      </c>
+      <c r="M100" s="51" t="s">
         <v>515</v>
       </c>
-      <c r="I100" s="1" t="s">
+      <c r="O100" s="51">
+        <v>9312</v>
+      </c>
+      <c r="P100" s="51" t="s">
+        <v>516</v>
+      </c>
+      <c r="Q100" s="51">
+        <v>3600</v>
+      </c>
+      <c r="R100" s="51">
+        <v>43.651156999999898</v>
+      </c>
+      <c r="S100" s="51">
+        <v>-79.476039999999898</v>
+      </c>
+      <c r="AG100" s="51" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="101" spans="1:33" s="51" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="51" t="s">
+        <v>652</v>
+      </c>
+      <c r="B101" s="52" t="s">
+        <v>669</v>
+      </c>
+      <c r="C101" s="53" t="s">
+        <v>146</v>
+      </c>
+      <c r="D101" s="51" t="s">
+        <v>515</v>
+      </c>
+      <c r="F101" s="51">
+        <v>9312</v>
+      </c>
+      <c r="G101" s="51" t="s">
+        <v>516</v>
+      </c>
+      <c r="H101" s="51" t="s">
+        <v>666</v>
+      </c>
+      <c r="I101" s="51" t="s">
+        <v>667</v>
+      </c>
+      <c r="J101" s="51">
+        <v>300</v>
+      </c>
+      <c r="K101" s="51">
+        <v>43.651156999999898</v>
+      </c>
+      <c r="L101" s="51">
+        <v>-79.476039999999898</v>
+      </c>
+      <c r="M101" s="51" t="s">
+        <v>665</v>
+      </c>
+      <c r="O101" s="51">
+        <v>5819</v>
+      </c>
+      <c r="P101" s="51" t="s">
+        <v>678</v>
+      </c>
+      <c r="Q101" s="51">
+        <v>3600</v>
+      </c>
+      <c r="R101" s="51">
+        <v>43.653686999999998</v>
+      </c>
+      <c r="S101" s="51">
+        <v>-79.465096000000003</v>
+      </c>
+      <c r="AG101" s="51" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="102" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B102" s="19" t="s">
+        <v>525</v>
+      </c>
+      <c r="C102" s="20" t="s">
         <v>517</v>
-      </c>
-      <c r="J100" s="1">
-        <v>300</v>
-      </c>
-      <c r="K100" s="1">
-        <v>43.656353600000003</v>
-      </c>
-      <c r="L100" s="1">
-        <v>-79.452438400000005</v>
-      </c>
-      <c r="M100" s="1" t="s">
-        <v>516</v>
-      </c>
-      <c r="O100" s="1">
-        <v>9312</v>
-      </c>
-      <c r="P100" s="1" t="s">
-        <v>519</v>
-      </c>
-      <c r="Q100" s="1">
-        <v>3600</v>
-      </c>
-      <c r="R100" s="1">
-        <v>43.651156999999898</v>
-      </c>
-      <c r="S100" s="1">
-        <v>-79.476039999999898</v>
-      </c>
-      <c r="AG100" s="47" t="s">
-        <v>674</v>
-      </c>
-    </row>
-    <row r="101" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A101" s="47" t="s">
-        <v>681</v>
-      </c>
-      <c r="B101" s="19" t="s">
-        <v>534</v>
-      </c>
-      <c r="C101" s="20" t="s">
-        <v>146</v>
-      </c>
-      <c r="D101" s="1" t="s">
-        <v>516</v>
-      </c>
-      <c r="F101" s="1">
-        <v>9312</v>
-      </c>
-      <c r="G101" s="1" t="s">
-        <v>519</v>
-      </c>
-      <c r="H101" s="1" t="s">
-        <v>518</v>
-      </c>
-      <c r="I101" s="1" t="s">
-        <v>520</v>
-      </c>
-      <c r="J101" s="1">
-        <v>300</v>
-      </c>
-      <c r="K101" s="1">
-        <v>43.651156999999898</v>
-      </c>
-      <c r="L101" s="1">
-        <v>-79.476039999999898</v>
-      </c>
-      <c r="M101" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="O101" s="1">
-        <v>5268</v>
-      </c>
-      <c r="P101" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="Q101" s="1">
-        <v>3600</v>
-      </c>
-      <c r="R101" s="1">
-        <v>43.656353600000003</v>
-      </c>
-      <c r="S101" s="1">
-        <v>-79.452438400000005</v>
-      </c>
-      <c r="AG101" s="47" t="s">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="102" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="B102" s="19" t="s">
-        <v>529</v>
-      </c>
-      <c r="C102" s="20" t="s">
-        <v>521</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>35</v>
@@ -8045,13 +8048,13 @@
         <v>9039</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="I102" s="1" t="s">
-        <v>640</v>
+        <v>634</v>
       </c>
       <c r="J102" s="1">
         <v>300</v>
@@ -8069,7 +8072,7 @@
         <v>5412</v>
       </c>
       <c r="P102" s="1" t="s">
-        <v>632</v>
+        <v>626</v>
       </c>
       <c r="Q102" s="1">
         <v>3600</v>
@@ -8081,12 +8084,12 @@
         <v>-79.432611499999894</v>
       </c>
     </row>
-    <row r="103" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="B103" s="19" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="C103" s="20" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>58</v>
@@ -8095,13 +8098,13 @@
         <v>5412</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>632</v>
+        <v>626</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="I103" s="1" t="s">
-        <v>554</v>
+        <v>548</v>
       </c>
       <c r="J103" s="1">
         <v>300</v>
@@ -8119,7 +8122,7 @@
         <v>9039</v>
       </c>
       <c r="P103" s="1" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="Q103" s="1">
         <v>3600</v>
@@ -8131,12 +8134,12 @@
         <v>-79.431478999999896</v>
       </c>
     </row>
-    <row r="104" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="B104" s="19" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="C104" s="20" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>58</v>
@@ -8145,13 +8148,13 @@
         <v>5412</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>632</v>
+        <v>626</v>
       </c>
       <c r="H104" s="1" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="I104" s="1" t="s">
-        <v>555</v>
+        <v>549</v>
       </c>
       <c r="J104" s="1">
         <v>300</v>
@@ -8181,12 +8184,12 @@
         <v>-79.435443899999896</v>
       </c>
     </row>
-    <row r="105" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="B105" s="19" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="C105" s="20" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>138</v>
@@ -8198,10 +8201,10 @@
         <v>150</v>
       </c>
       <c r="H105" s="1" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="I105" s="1" t="s">
-        <v>641</v>
+        <v>635</v>
       </c>
       <c r="J105" s="1">
         <v>300</v>
@@ -8219,7 +8222,7 @@
         <v>5412</v>
       </c>
       <c r="P105" s="1" t="s">
-        <v>632</v>
+        <v>626</v>
       </c>
       <c r="Q105" s="1">
         <v>3600</v>
@@ -8231,12 +8234,12 @@
         <v>-79.432611499999894</v>
       </c>
     </row>
-    <row r="106" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="B106" s="19" t="s">
-        <v>535</v>
+        <v>529</v>
       </c>
       <c r="C106" s="20" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>58</v>
@@ -8245,13 +8248,13 @@
         <v>5412</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>632</v>
+        <v>626</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
       <c r="I106" s="1" t="s">
-        <v>553</v>
+        <v>547</v>
       </c>
       <c r="J106" s="1">
         <v>300</v>
@@ -8269,7 +8272,7 @@
         <v>5272</v>
       </c>
       <c r="P106" s="1" t="s">
-        <v>633</v>
+        <v>627</v>
       </c>
       <c r="Q106" s="1">
         <v>3600</v>
@@ -8281,12 +8284,12 @@
         <v>-79.422612200000003</v>
       </c>
     </row>
-    <row r="107" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="B107" s="19" t="s">
-        <v>539</v>
+        <v>533</v>
       </c>
       <c r="C107" s="20" t="s">
-        <v>540</v>
+        <v>534</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>59</v>
@@ -8295,13 +8298,13 @@
         <v>5272</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>538</v>
+        <v>532</v>
       </c>
       <c r="H107" s="1" t="s">
-        <v>541</v>
+        <v>535</v>
       </c>
       <c r="I107" s="1" t="s">
-        <v>642</v>
+        <v>636</v>
       </c>
       <c r="J107" s="1">
         <v>300</v>
@@ -8319,7 +8322,7 @@
         <v>5412</v>
       </c>
       <c r="P107" s="1" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="Q107" s="1">
         <v>3600</v>
@@ -8331,12 +8334,12 @@
         <v>-79.432611499999894</v>
       </c>
     </row>
-    <row r="108" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="B108" s="19" t="s">
-        <v>542</v>
+        <v>536</v>
       </c>
       <c r="C108" s="20" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>59</v>
@@ -8345,13 +8348,13 @@
         <v>5272</v>
       </c>
       <c r="G108" s="1" t="s">
+        <v>532</v>
+      </c>
+      <c r="H108" s="1" t="s">
         <v>538</v>
       </c>
-      <c r="H108" s="1" t="s">
-        <v>544</v>
-      </c>
       <c r="I108" s="1" t="s">
-        <v>643</v>
+        <v>637</v>
       </c>
       <c r="J108" s="1">
         <v>300</v>
@@ -8369,7 +8372,7 @@
         <v>9098</v>
       </c>
       <c r="P108" s="1" t="s">
-        <v>545</v>
+        <v>539</v>
       </c>
       <c r="Q108" s="1">
         <v>3600</v>
@@ -8381,12 +8384,12 @@
         <v>-79.425572900000006</v>
       </c>
     </row>
-    <row r="109" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="B109" s="19" t="s">
-        <v>546</v>
+        <v>540</v>
       </c>
       <c r="C109" s="20" t="s">
-        <v>547</v>
+        <v>541</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>141</v>
@@ -8395,13 +8398,13 @@
         <v>9098</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>545</v>
+        <v>539</v>
       </c>
       <c r="H109" s="1" t="s">
-        <v>548</v>
+        <v>542</v>
       </c>
       <c r="I109" s="1" t="s">
-        <v>644</v>
+        <v>638</v>
       </c>
       <c r="J109" s="1">
         <v>300</v>
@@ -8419,7 +8422,7 @@
         <v>5272</v>
       </c>
       <c r="P109" s="1" t="s">
-        <v>538</v>
+        <v>532</v>
       </c>
       <c r="Q109" s="1">
         <v>3600</v>
@@ -8431,12 +8434,12 @@
         <v>-79.422612200000003</v>
       </c>
     </row>
-    <row r="110" spans="1:33" s="43" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:33" s="43" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="B110" s="41" t="s">
-        <v>549</v>
+        <v>543</v>
       </c>
       <c r="C110" s="42" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="D110" s="43" t="s">
         <v>28</v>
@@ -8448,10 +8451,10 @@
         <v>147</v>
       </c>
       <c r="H110" s="43" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="I110" s="43" t="s">
-        <v>552</v>
+        <v>546</v>
       </c>
       <c r="J110" s="43">
         <v>300</v>
@@ -8469,7 +8472,7 @@
         <v>9090</v>
       </c>
       <c r="P110" s="43" t="s">
-        <v>556</v>
+        <v>550</v>
       </c>
       <c r="Q110" s="43">
         <v>3600</v>
@@ -8481,12 +8484,12 @@
         <v>-79.4097376</v>
       </c>
     </row>
-    <row r="111" spans="1:33" s="43" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:33" s="43" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="B111" s="41" t="s">
-        <v>557</v>
+        <v>551</v>
       </c>
       <c r="C111" s="42" t="s">
-        <v>558</v>
+        <v>552</v>
       </c>
       <c r="D111" s="43" t="s">
         <v>71</v>
@@ -8495,13 +8498,13 @@
         <v>9090</v>
       </c>
       <c r="G111" s="43" t="s">
-        <v>556</v>
+        <v>550</v>
       </c>
       <c r="H111" s="43" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
       <c r="I111" s="43" t="s">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="J111" s="43">
         <v>300</v>
@@ -8531,12 +8534,12 @@
         <v>-79.407966000000002</v>
       </c>
     </row>
-    <row r="112" spans="1:33" s="43" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:33" s="43" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="B112" s="41" t="s">
-        <v>561</v>
+        <v>555</v>
       </c>
       <c r="C112" s="42" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="D112" s="43" t="s">
         <v>71</v>
@@ -8545,13 +8548,13 @@
         <v>9090</v>
       </c>
       <c r="G112" s="43" t="s">
+        <v>550</v>
+      </c>
+      <c r="H112" s="43" t="s">
         <v>556</v>
       </c>
-      <c r="H112" s="43" t="s">
-        <v>562</v>
-      </c>
       <c r="I112" s="43" t="s">
-        <v>563</v>
+        <v>557</v>
       </c>
       <c r="J112" s="43">
         <v>300</v>
@@ -8569,7 +8572,7 @@
         <v>9092</v>
       </c>
       <c r="P112" s="43" t="s">
-        <v>564</v>
+        <v>558</v>
       </c>
       <c r="Q112" s="43">
         <v>3600</v>
@@ -8581,12 +8584,12 @@
         <v>-79.411196700000005</v>
       </c>
     </row>
-    <row r="113" spans="2:19" s="43" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:19" s="43" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="B113" s="41" t="s">
-        <v>565</v>
+        <v>559</v>
       </c>
       <c r="C113" s="42" t="s">
-        <v>558</v>
+        <v>552</v>
       </c>
       <c r="D113" s="43" t="s">
         <v>136</v>
@@ -8595,13 +8598,13 @@
         <v>9092</v>
       </c>
       <c r="G113" s="43" t="s">
-        <v>564</v>
+        <v>558</v>
       </c>
       <c r="H113" s="43" t="s">
-        <v>566</v>
+        <v>560</v>
       </c>
       <c r="I113" s="43" t="s">
-        <v>618</v>
+        <v>612</v>
       </c>
       <c r="J113" s="43">
         <v>300</v>
@@ -8619,7 +8622,7 @@
         <v>9090</v>
       </c>
       <c r="P113" s="43" t="s">
-        <v>556</v>
+        <v>550</v>
       </c>
       <c r="Q113" s="43">
         <v>3600</v>
@@ -8631,12 +8634,12 @@
         <v>-79.4097376</v>
       </c>
     </row>
-    <row r="114" spans="2:19" s="43" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:19" s="43" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="B114" s="41" t="s">
-        <v>575</v>
+        <v>569</v>
       </c>
       <c r="C114" s="42" t="s">
-        <v>567</v>
+        <v>561</v>
       </c>
       <c r="D114" s="43" t="s">
         <v>60</v>
@@ -8645,13 +8648,13 @@
         <v>9093</v>
       </c>
       <c r="G114" s="43" t="s">
-        <v>568</v>
+        <v>562</v>
       </c>
       <c r="H114" s="43" t="s">
-        <v>569</v>
+        <v>563</v>
       </c>
       <c r="I114" s="43" t="s">
-        <v>570</v>
+        <v>564</v>
       </c>
       <c r="J114" s="43">
         <v>300</v>
@@ -8669,7 +8672,7 @@
         <v>9100</v>
       </c>
       <c r="P114" s="43" t="s">
-        <v>572</v>
+        <v>566</v>
       </c>
       <c r="Q114" s="43">
         <v>3600</v>
@@ -8681,12 +8684,12 @@
         <v>-79.402141599999894</v>
       </c>
     </row>
-    <row r="115" spans="2:19" s="43" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:19" s="43" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="B115" s="41" t="s">
-        <v>576</v>
+        <v>570</v>
       </c>
       <c r="C115" s="42" t="s">
-        <v>571</v>
+        <v>565</v>
       </c>
       <c r="D115" s="43" t="s">
         <v>72</v>
@@ -8695,13 +8698,13 @@
         <v>9100</v>
       </c>
       <c r="G115" s="43" t="s">
-        <v>572</v>
+        <v>566</v>
       </c>
       <c r="H115" s="43" t="s">
-        <v>574</v>
+        <v>568</v>
       </c>
       <c r="I115" s="43" t="s">
-        <v>573</v>
+        <v>567</v>
       </c>
       <c r="J115" s="43">
         <v>300</v>
@@ -8719,7 +8722,7 @@
         <v>9093</v>
       </c>
       <c r="P115" s="43" t="s">
-        <v>568</v>
+        <v>562</v>
       </c>
       <c r="Q115" s="43">
         <v>3600</v>
@@ -8731,12 +8734,12 @@
         <v>-79.400038699999897</v>
       </c>
     </row>
-    <row r="116" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B116" s="19" t="s">
-        <v>577</v>
+        <v>571</v>
       </c>
       <c r="C116" s="20" t="s">
-        <v>567</v>
+        <v>561</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>72</v>
@@ -8745,13 +8748,13 @@
         <v>9100</v>
       </c>
       <c r="G116" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="H116" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="I116" s="1" t="s">
         <v>572</v>
-      </c>
-      <c r="H116" s="1" t="s">
-        <v>580</v>
-      </c>
-      <c r="I116" s="1" t="s">
-        <v>578</v>
       </c>
       <c r="J116" s="1">
         <v>300</v>
@@ -8781,12 +8784,12 @@
         <v>-79.403815300000005</v>
       </c>
     </row>
-    <row r="117" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="117" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B117" s="19" t="s">
-        <v>579</v>
+        <v>573</v>
       </c>
       <c r="C117" s="20" t="s">
-        <v>571</v>
+        <v>565</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>143</v>
@@ -8798,10 +8801,10 @@
         <v>162</v>
       </c>
       <c r="H117" s="1" t="s">
-        <v>581</v>
+        <v>575</v>
       </c>
       <c r="I117" s="1" t="s">
-        <v>582</v>
+        <v>576</v>
       </c>
       <c r="J117" s="1">
         <v>300</v>
@@ -8819,7 +8822,7 @@
         <v>9100</v>
       </c>
       <c r="P117" s="1" t="s">
-        <v>572</v>
+        <v>566</v>
       </c>
       <c r="Q117" s="1">
         <v>3600</v>
@@ -8831,12 +8834,12 @@
         <v>-79.402141599999894</v>
       </c>
     </row>
-    <row r="118" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="118" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B118" s="19" t="s">
-        <v>586</v>
+        <v>580</v>
       </c>
       <c r="C118" s="20" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
       <c r="D118" s="1" t="s">
         <v>71</v>
@@ -8845,13 +8848,13 @@
         <v>9090</v>
       </c>
       <c r="G118" s="43" t="s">
-        <v>556</v>
+        <v>550</v>
       </c>
       <c r="H118" s="43" t="s">
+        <v>578</v>
+      </c>
+      <c r="I118" s="43" t="s">
         <v>584</v>
-      </c>
-      <c r="I118" s="43" t="s">
-        <v>590</v>
       </c>
       <c r="J118" s="43">
         <v>300</v>
@@ -8869,7 +8872,7 @@
         <v>9100</v>
       </c>
       <c r="P118" s="1" t="s">
-        <v>572</v>
+        <v>566</v>
       </c>
       <c r="Q118" s="1">
         <v>3600</v>
@@ -8881,12 +8884,12 @@
         <v>-79.402141599999894</v>
       </c>
     </row>
-    <row r="119" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="119" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B119" s="19" t="s">
-        <v>585</v>
+        <v>579</v>
       </c>
       <c r="C119" s="20" t="s">
-        <v>587</v>
+        <v>581</v>
       </c>
       <c r="D119" s="1" t="s">
         <v>72</v>
@@ -8895,13 +8898,13 @@
         <v>9100</v>
       </c>
       <c r="G119" s="1" t="s">
-        <v>572</v>
+        <v>566</v>
       </c>
       <c r="H119" s="43" t="s">
-        <v>588</v>
+        <v>582</v>
       </c>
       <c r="I119" s="1" t="s">
-        <v>589</v>
+        <v>583</v>
       </c>
       <c r="J119" s="1">
         <v>300</v>
@@ -8919,7 +8922,7 @@
         <v>9090</v>
       </c>
       <c r="P119" s="43" t="s">
-        <v>556</v>
+        <v>550</v>
       </c>
       <c r="Q119" s="1">
         <v>3600</v>
@@ -8931,12 +8934,12 @@
         <v>-79.4097376</v>
       </c>
     </row>
-    <row r="120" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="120" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B120" s="19" t="s">
-        <v>591</v>
+        <v>585</v>
       </c>
       <c r="C120" s="20" t="s">
-        <v>583</v>
+        <v>577</v>
       </c>
       <c r="D120" s="1" t="s">
         <v>72</v>
@@ -8945,13 +8948,13 @@
         <v>9100</v>
       </c>
       <c r="G120" s="1" t="s">
-        <v>572</v>
+        <v>566</v>
       </c>
       <c r="H120" s="43" t="s">
-        <v>594</v>
+        <v>588</v>
       </c>
       <c r="I120" s="1" t="s">
-        <v>595</v>
+        <v>589</v>
       </c>
       <c r="J120" s="1">
         <v>300</v>
@@ -8969,7 +8972,7 @@
         <v>5612</v>
       </c>
       <c r="P120" s="1" t="s">
-        <v>592</v>
+        <v>586</v>
       </c>
       <c r="Q120" s="1">
         <v>3600</v>
@@ -8981,12 +8984,12 @@
         <v>-79.393966199999895</v>
       </c>
     </row>
-    <row r="121" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="121" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B121" s="19" t="s">
-        <v>593</v>
+        <v>587</v>
       </c>
       <c r="C121" s="20" t="s">
-        <v>647</v>
+        <v>641</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>84</v>
@@ -8995,13 +8998,13 @@
         <v>5612</v>
       </c>
       <c r="G121" s="1" t="s">
-        <v>592</v>
+        <v>586</v>
       </c>
       <c r="H121" s="1" t="s">
-        <v>596</v>
+        <v>590</v>
       </c>
       <c r="I121" s="1" t="s">
-        <v>597</v>
+        <v>591</v>
       </c>
       <c r="J121" s="1">
         <v>300</v>
@@ -9019,7 +9022,7 @@
         <v>9100</v>
       </c>
       <c r="P121" s="1" t="s">
-        <v>572</v>
+        <v>566</v>
       </c>
       <c r="Q121" s="1">
         <v>3600</v>
@@ -9031,12 +9034,12 @@
         <v>-79.402141599999894</v>
       </c>
     </row>
-    <row r="122" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B122" s="1" t="s">
-        <v>609</v>
+        <v>603</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>598</v>
+        <v>592</v>
       </c>
       <c r="D122" s="1" t="s">
         <v>30</v>
@@ -9045,13 +9048,13 @@
         <v>5414</v>
       </c>
       <c r="G122" s="1" t="s">
-        <v>599</v>
+        <v>593</v>
       </c>
       <c r="H122" s="1" t="s">
-        <v>610</v>
+        <v>604</v>
       </c>
       <c r="I122" s="1" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="J122" s="1">
         <v>300</v>
@@ -9069,7 +9072,7 @@
         <v>9097</v>
       </c>
       <c r="P122" s="1" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
       <c r="Q122" s="1">
         <v>3600</v>
@@ -9081,12 +9084,12 @@
         <v>-79.390618799999899</v>
       </c>
     </row>
-    <row r="123" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="123" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B123" s="1" t="s">
-        <v>600</v>
+        <v>594</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>601</v>
+        <v>595</v>
       </c>
       <c r="D123" s="1" t="s">
         <v>84</v>
@@ -9095,13 +9098,13 @@
         <v>5612</v>
       </c>
       <c r="G123" s="1" t="s">
-        <v>592</v>
+        <v>586</v>
       </c>
       <c r="H123" s="1" t="s">
-        <v>602</v>
+        <v>596</v>
       </c>
       <c r="I123" s="1" t="s">
-        <v>603</v>
+        <v>597</v>
       </c>
       <c r="J123" s="1">
         <v>300</v>
@@ -9119,7 +9122,7 @@
         <v>5414</v>
       </c>
       <c r="P123" s="1" t="s">
-        <v>599</v>
+        <v>593</v>
       </c>
       <c r="Q123" s="1">
         <v>3600</v>
@@ -9131,12 +9134,12 @@
         <v>-79.390716999999896</v>
       </c>
     </row>
-    <row r="124" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="124" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B124" s="40" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="C124" s="40" t="s">
-        <v>598</v>
+        <v>592</v>
       </c>
       <c r="D124" s="40" t="s">
         <v>78</v>
@@ -9146,13 +9149,13 @@
         <v>9097</v>
       </c>
       <c r="G124" s="40" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
       <c r="H124" s="40" t="s">
-        <v>614</v>
+        <v>608</v>
       </c>
       <c r="I124" s="40" t="s">
-        <v>615</v>
+        <v>609</v>
       </c>
       <c r="J124" s="40">
         <v>300</v>
@@ -9183,12 +9186,12 @@
         <v>-79.394137900000004</v>
       </c>
     </row>
-    <row r="125" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="125" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B125" s="19" t="s">
-        <v>612</v>
+        <v>606</v>
       </c>
       <c r="C125" s="20" t="s">
-        <v>601</v>
+        <v>595</v>
       </c>
       <c r="D125" s="1" t="s">
         <v>135</v>
@@ -9200,10 +9203,10 @@
         <v>166</v>
       </c>
       <c r="H125" s="1" t="s">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="I125" s="1" t="s">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="J125" s="1">
         <v>300</v>
@@ -9221,7 +9224,7 @@
         <v>5612</v>
       </c>
       <c r="P125" s="1" t="s">
-        <v>592</v>
+        <v>586</v>
       </c>
       <c r="Q125" s="1">
         <v>3600</v>
@@ -9233,12 +9236,12 @@
         <v>-79.393966199999895</v>
       </c>
     </row>
-    <row r="126" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="126" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B126" s="19" t="s">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="C126" s="20" t="s">
-        <v>608</v>
+        <v>602</v>
       </c>
       <c r="D126" s="43" t="s">
         <v>78</v>
@@ -9248,13 +9251,13 @@
         <v>9097</v>
       </c>
       <c r="G126" s="43" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
       <c r="H126" s="43" t="s">
-        <v>616</v>
+        <v>610</v>
       </c>
       <c r="I126" s="43" t="s">
-        <v>617</v>
+        <v>611</v>
       </c>
       <c r="J126" s="43">
         <v>300</v>
@@ -9284,12 +9287,12 @@
         <v>-79.3845034</v>
       </c>
     </row>
-    <row r="127" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="127" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B127" s="19" t="s">
-        <v>619</v>
+        <v>613</v>
       </c>
       <c r="C127" s="20" t="s">
-        <v>620</v>
+        <v>614</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>79</v>
@@ -9301,10 +9304,10 @@
         <v>440</v>
       </c>
       <c r="H127" s="43" t="s">
-        <v>621</v>
+        <v>615</v>
       </c>
       <c r="I127" s="43" t="s">
-        <v>622</v>
+        <v>616</v>
       </c>
       <c r="J127" s="43">
         <v>300</v>
@@ -9323,7 +9326,7 @@
         <v>9097</v>
       </c>
       <c r="P127" s="43" t="s">
-        <v>604</v>
+        <v>598</v>
       </c>
       <c r="Q127" s="1">
         <v>3600</v>
@@ -9335,12 +9338,12 @@
         <v>-79.393966199999895</v>
       </c>
     </row>
-    <row r="128" spans="2:19" x14ac:dyDescent="0.2">
+    <row r="128" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="B128" s="19" t="s">
-        <v>623</v>
+        <v>617</v>
       </c>
       <c r="C128" s="20" t="s">
-        <v>608</v>
+        <v>602</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>79</v>
@@ -9352,10 +9355,10 @@
         <v>440</v>
       </c>
       <c r="H128" s="43" t="s">
-        <v>624</v>
+        <v>618</v>
       </c>
       <c r="I128" s="43" t="s">
-        <v>625</v>
+        <v>619</v>
       </c>
       <c r="J128" s="43">
         <v>300</v>
@@ -9385,12 +9388,12 @@
         <v>-79.378280599999897</v>
       </c>
     </row>
-    <row r="129" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="B129" s="19" t="s">
-        <v>626</v>
+        <v>620</v>
       </c>
       <c r="C129" s="20" t="s">
-        <v>620</v>
+        <v>614</v>
       </c>
       <c r="D129" s="1" t="s">
         <v>77</v>
@@ -9402,10 +9405,10 @@
         <v>405</v>
       </c>
       <c r="H129" s="43" t="s">
-        <v>627</v>
+        <v>621</v>
       </c>
       <c r="I129" s="43" t="s">
-        <v>628</v>
+        <v>622</v>
       </c>
       <c r="J129" s="1">
         <v>300</v>
@@ -9435,12 +9438,12 @@
         <v>-79.3845034</v>
       </c>
     </row>
-    <row r="130" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="B130" s="19" t="s">
-        <v>629</v>
+        <v>623</v>
       </c>
       <c r="C130" s="20" t="s">
-        <v>608</v>
+        <v>602</v>
       </c>
       <c r="D130" s="1" t="s">
         <v>77</v>
@@ -9452,10 +9455,10 @@
         <v>405</v>
       </c>
       <c r="H130" s="43" t="s">
-        <v>627</v>
+        <v>621</v>
       </c>
       <c r="I130" s="43" t="s">
-        <v>630</v>
+        <v>624</v>
       </c>
       <c r="J130" s="1">
         <v>300</v>
@@ -9485,12 +9488,12 @@
         <v>-79.369504500000005</v>
       </c>
     </row>
-    <row r="131" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="B131" s="19" t="s">
-        <v>631</v>
+        <v>625</v>
       </c>
       <c r="C131" s="20" t="s">
-        <v>620</v>
+        <v>614</v>
       </c>
       <c r="D131" s="1" t="s">
         <v>86</v>
@@ -9502,10 +9505,10 @@
         <v>421</v>
       </c>
       <c r="H131" s="43" t="s">
-        <v>624</v>
+        <v>618</v>
       </c>
       <c r="I131" s="43" t="s">
-        <v>645</v>
+        <v>639</v>
       </c>
       <c r="J131" s="1">
         <v>300</v>
@@ -9535,12 +9538,12 @@
         <v>-79.378280599999897</v>
       </c>
     </row>
-    <row r="132" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="B132" s="19" t="s">
-        <v>636</v>
+        <v>630</v>
       </c>
       <c r="C132" s="20" t="s">
-        <v>547</v>
+        <v>541</v>
       </c>
       <c r="D132" s="1" t="s">
         <v>59</v>
@@ -9549,13 +9552,13 @@
         <v>5272</v>
       </c>
       <c r="G132" s="1" t="s">
-        <v>538</v>
+        <v>532</v>
       </c>
       <c r="H132" s="1" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="I132" s="1" t="s">
-        <v>635</v>
+        <v>629</v>
       </c>
       <c r="J132" s="1">
         <v>300</v>
@@ -9585,12 +9588,12 @@
         <v>-79.420862700000001</v>
       </c>
     </row>
-    <row r="133" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="B133" s="19" t="s">
-        <v>637</v>
+        <v>631</v>
       </c>
       <c r="C133" s="20" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
       <c r="D133" s="1" t="s">
         <v>64</v>
@@ -9602,10 +9605,10 @@
         <v>417</v>
       </c>
       <c r="H133" s="1" t="s">
-        <v>638</v>
+        <v>632</v>
       </c>
       <c r="I133" s="1" t="s">
-        <v>639</v>
+        <v>633</v>
       </c>
       <c r="J133" s="1">
         <v>300</v>
@@ -9623,7 +9626,7 @@
         <v>5272</v>
       </c>
       <c r="P133" s="1" t="s">
-        <v>538</v>
+        <v>532</v>
       </c>
       <c r="Q133" s="1">
         <v>3600</v>
@@ -9635,779 +9638,542 @@
         <v>-79.422612200000003</v>
       </c>
     </row>
-    <row r="134" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A134" s="47" t="s">
+    <row r="134" spans="1:33" s="51" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A134" s="51" t="s">
+        <v>652</v>
+      </c>
+      <c r="B134" s="52" t="s">
+        <v>673</v>
+      </c>
+      <c r="C134" s="53" t="s">
+        <v>146</v>
+      </c>
+      <c r="D134" s="51" t="s">
+        <v>665</v>
+      </c>
+      <c r="F134" s="51">
+        <v>5819</v>
+      </c>
+      <c r="G134" s="51" t="s">
+        <v>678</v>
+      </c>
+      <c r="H134" s="51" t="s">
+        <v>674</v>
+      </c>
+      <c r="I134" s="51" t="s">
+        <v>675</v>
+      </c>
+      <c r="J134" s="51">
+        <v>300</v>
+      </c>
+      <c r="K134" s="51">
+        <v>43.653686999999998</v>
+      </c>
+      <c r="L134" s="51">
+        <v>-79.465096000000003</v>
+      </c>
+      <c r="M134" s="51" t="s">
+        <v>138</v>
+      </c>
+      <c r="O134" s="51">
+        <v>9096</v>
+      </c>
+      <c r="P134" s="51" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q134" s="51">
+        <v>3600</v>
+      </c>
+      <c r="R134" s="51">
+        <v>43.659861999999997</v>
+      </c>
+      <c r="S134" s="51">
+        <v>-79.435443899999996</v>
+      </c>
+      <c r="AG134" s="51" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="135" spans="1:33" s="51" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A135" s="51" t="s">
+        <v>652</v>
+      </c>
+      <c r="B135" s="52" t="s">
+        <v>679</v>
+      </c>
+      <c r="C135" s="53" t="s">
+        <v>287</v>
+      </c>
+      <c r="D135" s="51" t="s">
+        <v>138</v>
+      </c>
+      <c r="F135" s="51">
+        <v>9096</v>
+      </c>
+      <c r="G135" s="51" t="s">
+        <v>150</v>
+      </c>
+      <c r="H135" s="51" t="s">
+        <v>676</v>
+      </c>
+      <c r="I135" s="51" t="s">
+        <v>677</v>
+      </c>
+      <c r="J135" s="51">
+        <v>300</v>
+      </c>
+      <c r="K135" s="51">
+        <v>43.659861999999997</v>
+      </c>
+      <c r="L135" s="51">
+        <v>-79.435443899999996</v>
+      </c>
+      <c r="M135" s="51" t="s">
+        <v>665</v>
+      </c>
+      <c r="O135" s="51">
+        <v>5819</v>
+      </c>
+      <c r="P135" s="51" t="s">
+        <v>678</v>
+      </c>
+      <c r="Q135" s="51">
+        <v>3600</v>
+      </c>
+      <c r="R135" s="51">
+        <v>43.653686999999998</v>
+      </c>
+      <c r="S135" s="51">
+        <v>-79.465096000000003</v>
+      </c>
+      <c r="AG135" s="51" t="s">
         <v>681</v>
       </c>
-      <c r="B134" s="19" t="s">
-        <v>652</v>
-      </c>
-      <c r="C134" s="20" t="s">
-        <v>146</v>
-      </c>
-      <c r="D134" s="1" t="s">
+    </row>
+    <row r="136" spans="1:33" s="43" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A136" s="48" t="s">
+        <v>653</v>
+      </c>
+      <c r="B136" s="49" t="s">
+        <v>682</v>
+      </c>
+      <c r="C136" s="50" t="s">
+        <v>517</v>
+      </c>
+      <c r="D136" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="E136" s="48"/>
+      <c r="F136" s="48">
+        <v>9039</v>
+      </c>
+      <c r="G136" s="48" t="s">
+        <v>518</v>
+      </c>
+      <c r="H136" s="48" t="s">
+        <v>685</v>
+      </c>
+      <c r="I136" s="48" t="s">
+        <v>686</v>
+      </c>
+      <c r="J136" s="48">
+        <v>300</v>
+      </c>
+      <c r="K136" s="48">
+        <v>43.6495409999999</v>
+      </c>
+      <c r="L136" s="48">
+        <v>-79.431478999999896</v>
+      </c>
+      <c r="M136" s="48" t="s">
+        <v>138</v>
+      </c>
+      <c r="N136" s="48"/>
+      <c r="O136" s="48">
+        <v>9096</v>
+      </c>
+      <c r="P136" s="48" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q136" s="48">
+        <v>3600</v>
+      </c>
+      <c r="R136" s="48">
+        <v>43.659861999999997</v>
+      </c>
+      <c r="S136" s="48">
+        <v>-79.435443899999996</v>
+      </c>
+      <c r="T136" s="48"/>
+      <c r="U136" s="48"/>
+      <c r="V136" s="48"/>
+      <c r="W136" s="48"/>
+      <c r="X136" s="48"/>
+      <c r="Y136" s="48"/>
+      <c r="Z136" s="48"/>
+      <c r="AA136" s="48"/>
+      <c r="AB136" s="48"/>
+      <c r="AC136" s="48"/>
+      <c r="AD136" s="48"/>
+      <c r="AE136" s="48"/>
+      <c r="AF136" s="48"/>
+      <c r="AG136" s="48" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="137" spans="1:33" s="43" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A137" s="48" t="s">
+        <v>653</v>
+      </c>
+      <c r="B137" s="49" t="s">
+        <v>683</v>
+      </c>
+      <c r="C137" s="50" t="s">
+        <v>521</v>
+      </c>
+      <c r="D137" s="48" t="s">
+        <v>138</v>
+      </c>
+      <c r="E137" s="48"/>
+      <c r="F137" s="48">
+        <v>9096</v>
+      </c>
+      <c r="G137" s="48" t="s">
+        <v>150</v>
+      </c>
+      <c r="H137" s="48" t="s">
+        <v>684</v>
+      </c>
+      <c r="I137" s="48" t="s">
+        <v>687</v>
+      </c>
+      <c r="J137" s="48">
+        <v>300</v>
+      </c>
+      <c r="K137" s="48">
+        <v>43.659861999999997</v>
+      </c>
+      <c r="L137" s="48">
+        <v>-79.435443899999996</v>
+      </c>
+      <c r="M137" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="N137" s="48"/>
+      <c r="O137" s="48">
+        <v>9039</v>
+      </c>
+      <c r="P137" s="48" t="s">
+        <v>518</v>
+      </c>
+      <c r="Q137" s="48">
+        <v>3600</v>
+      </c>
+      <c r="R137" s="48">
+        <v>43.6495409999999</v>
+      </c>
+      <c r="S137" s="48">
+        <v>-79.431478999999896</v>
+      </c>
+      <c r="T137" s="48"/>
+      <c r="U137" s="48"/>
+      <c r="V137" s="48"/>
+      <c r="W137" s="48"/>
+      <c r="X137" s="48"/>
+      <c r="Y137" s="48"/>
+      <c r="Z137" s="48"/>
+      <c r="AA137" s="48"/>
+      <c r="AB137" s="48"/>
+      <c r="AC137" s="48"/>
+      <c r="AD137" s="48"/>
+      <c r="AE137" s="48"/>
+      <c r="AF137" s="48"/>
+      <c r="AG137" s="48" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="138" spans="1:33" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A138" s="47" t="s">
+        <v>642</v>
+      </c>
+      <c r="B138" s="54" t="s">
+        <v>645</v>
+      </c>
+      <c r="C138" s="55" t="s">
+        <v>510</v>
+      </c>
+      <c r="D138" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="F138" s="47">
+        <v>9021</v>
+      </c>
+      <c r="G138" s="47" t="s">
+        <v>646</v>
+      </c>
+      <c r="H138" s="47" t="s">
+        <v>647</v>
+      </c>
+      <c r="I138" s="47" t="s">
+        <v>648</v>
+      </c>
+      <c r="J138" s="47">
+        <v>300</v>
+      </c>
+      <c r="K138" s="47">
+        <v>43.638885000000002</v>
+      </c>
+      <c r="L138" s="47">
+        <v>-79.446359999999899</v>
+      </c>
+      <c r="M138" s="47" t="s">
         <v>139</v>
       </c>
-      <c r="F134" s="1">
+      <c r="O138" s="47">
         <v>5268</v>
       </c>
-      <c r="G134" s="1" t="s">
+      <c r="P138" s="47" t="s">
         <v>147</v>
       </c>
-      <c r="H134" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="I134" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="J134" s="1">
-        <v>300</v>
-      </c>
-      <c r="K134" s="1">
+      <c r="Q138" s="47">
+        <v>3600</v>
+      </c>
+      <c r="R138" s="47">
         <v>43.656353600000003</v>
       </c>
-      <c r="L134" s="1">
+      <c r="S138" s="47">
         <v>-79.452438400000005</v>
       </c>
-      <c r="M134" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="O134" s="1">
-        <v>9096</v>
-      </c>
-      <c r="P134" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="Q134" s="1">
-        <v>3600</v>
-      </c>
-      <c r="R134" s="1">
-        <v>43.659861999999997</v>
-      </c>
-      <c r="S134" s="1">
-        <v>-79.435443899999996</v>
-      </c>
-      <c r="AG134" s="47" t="s">
-        <v>674</v>
-      </c>
-    </row>
-    <row r="135" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A135" s="47" t="s">
-        <v>681</v>
-      </c>
-      <c r="B135" s="19" t="s">
+      <c r="AG138" s="47" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="139" spans="1:33" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A139" s="47" t="s">
+        <v>642</v>
+      </c>
+      <c r="B139" s="54" t="s">
+        <v>649</v>
+      </c>
+      <c r="C139" s="55" t="s">
+        <v>512</v>
+      </c>
+      <c r="D139" s="47" t="s">
+        <v>139</v>
+      </c>
+      <c r="F139" s="47">
+        <v>5268</v>
+      </c>
+      <c r="G139" s="47" t="s">
+        <v>147</v>
+      </c>
+      <c r="H139" s="47" t="s">
+        <v>650</v>
+      </c>
+      <c r="I139" s="47" t="s">
+        <v>651</v>
+      </c>
+      <c r="J139" s="47">
+        <v>300</v>
+      </c>
+      <c r="K139" s="47">
+        <v>43.656353600000003</v>
+      </c>
+      <c r="L139" s="47">
+        <v>-79.452438400000005</v>
+      </c>
+      <c r="M139" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="O139" s="47">
+        <v>9021</v>
+      </c>
+      <c r="P139" s="47" t="s">
+        <v>646</v>
+      </c>
+      <c r="Q139" s="47">
+        <v>3600</v>
+      </c>
+      <c r="R139" s="47">
+        <v>43.638885000000002</v>
+      </c>
+      <c r="S139" s="47">
+        <v>-79.446359999999899</v>
+      </c>
+      <c r="AG139" s="47" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="140" spans="1:33" s="51" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A140" s="51" t="s">
+        <v>642</v>
+      </c>
+      <c r="B140" s="52" t="s">
         <v>654</v>
       </c>
-      <c r="C135" s="20" t="s">
-        <v>287</v>
-      </c>
-      <c r="D135" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F135" s="1">
-        <v>9096</v>
-      </c>
-      <c r="G135" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="H135" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="I135" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="J135" s="1">
-        <v>300</v>
-      </c>
-      <c r="K135" s="1">
-        <v>43.659861999999997</v>
-      </c>
-      <c r="L135" s="1">
-        <v>-79.435443899999996</v>
-      </c>
-      <c r="M135" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="O135" s="1">
-        <v>5268</v>
-      </c>
-      <c r="P135" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="Q135" s="1">
-        <v>3600</v>
-      </c>
-      <c r="R135" s="1">
-        <v>43.656353600000003</v>
-      </c>
-      <c r="S135" s="1">
-        <v>-79.452438400000005</v>
-      </c>
-      <c r="AG135" s="47" t="s">
-        <v>683</v>
-      </c>
-    </row>
-    <row r="136" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A136" s="47" t="s">
-        <v>681</v>
-      </c>
-      <c r="B136" s="19" t="s">
-        <v>653</v>
-      </c>
-      <c r="C136" s="20" t="s">
-        <v>146</v>
-      </c>
-      <c r="D136" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F136" s="1">
-        <v>9096</v>
-      </c>
-      <c r="G136" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="H136" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="I136" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="J136" s="1">
-        <v>300</v>
-      </c>
-      <c r="K136" s="1">
-        <v>43.659861999999997</v>
-      </c>
-      <c r="L136" s="1">
-        <v>-79.435443899999996</v>
-      </c>
-      <c r="M136" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="O136" s="1">
-        <v>9098</v>
-      </c>
-      <c r="P136" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q136" s="1">
-        <v>3600</v>
-      </c>
-      <c r="R136" s="1">
-        <v>43.661911099999998</v>
-      </c>
-      <c r="S136" s="1">
-        <v>-79.425572900000006</v>
-      </c>
-      <c r="AG136" s="47" t="s">
-        <v>683</v>
-      </c>
-    </row>
-    <row r="137" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A137" s="47" t="s">
-        <v>681</v>
-      </c>
-      <c r="B137" s="19" t="s">
+      <c r="C140" s="53" t="s">
         <v>655</v>
       </c>
-      <c r="C137" s="20" t="s">
-        <v>287</v>
-      </c>
-      <c r="D137" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="F137" s="1">
-        <v>9098</v>
-      </c>
-      <c r="G137" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="H137" s="1" t="s">
-        <v>306</v>
-      </c>
-      <c r="I137" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="J137" s="1">
-        <v>300</v>
-      </c>
-      <c r="K137" s="1">
-        <v>43.661911099999998</v>
-      </c>
-      <c r="L137" s="1">
-        <v>-79.425572900000006</v>
-      </c>
-      <c r="M137" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="O137" s="1">
-        <v>9096</v>
-      </c>
-      <c r="P137" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="Q137" s="1">
-        <v>3600</v>
-      </c>
-      <c r="R137" s="1">
-        <v>43.659861999999997</v>
-      </c>
-      <c r="S137" s="1">
-        <v>-79.435443899999996</v>
-      </c>
-      <c r="AG137" s="47" t="s">
+      <c r="D140" s="51" t="s">
+        <v>41</v>
+      </c>
+      <c r="F140" s="51">
+        <v>9038</v>
+      </c>
+      <c r="G140" s="51" t="s">
+        <v>658</v>
+      </c>
+      <c r="H140" s="51" t="s">
+        <v>659</v>
+      </c>
+      <c r="I140" s="51" t="s">
+        <v>660</v>
+      </c>
+      <c r="J140" s="51">
+        <v>300</v>
+      </c>
+      <c r="K140" s="51">
+        <v>43.654710000000001</v>
+      </c>
+      <c r="L140" s="51">
+        <v>-79.388576999999898</v>
+      </c>
+      <c r="M140" s="51" t="s">
+        <v>135</v>
+      </c>
+      <c r="O140" s="51">
+        <v>5330</v>
+      </c>
+      <c r="P140" s="51" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q140" s="51">
+        <v>3600</v>
+      </c>
+      <c r="R140" s="51">
+        <v>43.668709800000002</v>
+      </c>
+      <c r="S140" s="51">
+        <v>-79.394137900000004</v>
+      </c>
+      <c r="AG140" s="51" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="141" spans="1:33" s="51" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A141" s="51" t="s">
+        <v>642</v>
+      </c>
+      <c r="B141" s="52" t="s">
         <v>656</v>
       </c>
-    </row>
-    <row r="138" spans="1:33" s="48" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A138" s="47" t="s">
-        <v>681</v>
-      </c>
-      <c r="B138" s="41" t="s">
-        <v>666</v>
-      </c>
-      <c r="C138" s="42" t="s">
-        <v>510</v>
-      </c>
-      <c r="D138" s="43" t="s">
-        <v>49</v>
-      </c>
-      <c r="E138" s="43"/>
-      <c r="F138" s="43">
-        <v>9021</v>
-      </c>
-      <c r="G138" s="43" t="s">
-        <v>667</v>
-      </c>
-      <c r="H138" s="43" t="s">
-        <v>668</v>
-      </c>
-      <c r="I138" s="43" t="s">
-        <v>669</v>
-      </c>
-      <c r="J138" s="43">
-        <v>300</v>
-      </c>
-      <c r="K138" s="43">
-        <v>43.638885000000002</v>
-      </c>
-      <c r="L138" s="43">
-        <v>-79.446359999999899</v>
-      </c>
-      <c r="M138" s="43" t="s">
-        <v>139</v>
-      </c>
-      <c r="N138" s="43"/>
-      <c r="O138" s="43">
-        <v>5268</v>
-      </c>
-      <c r="P138" s="43" t="s">
-        <v>147</v>
-      </c>
-      <c r="Q138" s="43">
-        <v>3600</v>
-      </c>
-      <c r="R138" s="43">
-        <v>43.656353600000003</v>
-      </c>
-      <c r="S138" s="43">
-        <v>-79.452438400000005</v>
-      </c>
-      <c r="T138" s="43"/>
-      <c r="U138" s="43"/>
-      <c r="V138" s="43"/>
-      <c r="W138" s="43"/>
-      <c r="X138" s="43"/>
-      <c r="Y138" s="43"/>
-      <c r="Z138" s="43"/>
-      <c r="AA138" s="43"/>
-      <c r="AB138" s="43"/>
-      <c r="AC138" s="43"/>
-      <c r="AD138" s="43"/>
-      <c r="AE138" s="43"/>
-      <c r="AF138" s="43"/>
-      <c r="AG138" s="47" t="s">
+      <c r="C141" s="53" t="s">
         <v>657</v>
       </c>
-    </row>
-    <row r="139" spans="1:33" s="48" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A139" s="47" t="s">
-        <v>681</v>
-      </c>
-      <c r="B139" s="41" t="s">
-        <v>670</v>
-      </c>
-      <c r="C139" s="42" t="s">
-        <v>512</v>
-      </c>
-      <c r="D139" s="43" t="s">
-        <v>139</v>
-      </c>
-      <c r="E139" s="43"/>
-      <c r="F139" s="43">
-        <v>5268</v>
-      </c>
-      <c r="G139" s="43" t="s">
-        <v>147</v>
-      </c>
-      <c r="H139" s="43" t="s">
-        <v>671</v>
-      </c>
-      <c r="I139" s="43" t="s">
-        <v>672</v>
-      </c>
-      <c r="J139" s="43">
-        <v>300</v>
-      </c>
-      <c r="K139" s="43">
-        <v>43.656353600000003</v>
-      </c>
-      <c r="L139" s="43">
-        <v>-79.452438400000005</v>
-      </c>
-      <c r="M139" s="43" t="s">
-        <v>49</v>
-      </c>
-      <c r="N139" s="43"/>
-      <c r="O139" s="43">
-        <v>9021</v>
-      </c>
-      <c r="P139" s="43" t="s">
-        <v>667</v>
-      </c>
-      <c r="Q139" s="43">
-        <v>3600</v>
-      </c>
-      <c r="R139" s="43">
-        <v>43.638885000000002</v>
-      </c>
-      <c r="S139" s="43">
-        <v>-79.446359999999899</v>
-      </c>
-      <c r="T139" s="43"/>
-      <c r="U139" s="43"/>
-      <c r="V139" s="43"/>
-      <c r="W139" s="43"/>
-      <c r="X139" s="43"/>
-      <c r="Y139" s="43"/>
-      <c r="Z139" s="43"/>
-      <c r="AA139" s="43"/>
-      <c r="AB139" s="43"/>
-      <c r="AC139" s="43"/>
-      <c r="AD139" s="43"/>
-      <c r="AE139" s="43"/>
-      <c r="AF139" s="43"/>
-      <c r="AG139" s="47" t="s">
-        <v>657</v>
-      </c>
-    </row>
-    <row r="140" spans="1:33" s="48" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A140" s="48" t="s">
-        <v>682</v>
-      </c>
-      <c r="B140" s="49" t="s">
+      <c r="D141" s="51" t="s">
+        <v>135</v>
+      </c>
+      <c r="F141" s="51">
+        <v>5330</v>
+      </c>
+      <c r="G141" s="51" t="s">
+        <v>166</v>
+      </c>
+      <c r="H141" s="51" t="s">
+        <v>661</v>
+      </c>
+      <c r="I141" s="51" t="s">
+        <v>662</v>
+      </c>
+      <c r="J141" s="51">
+        <v>300</v>
+      </c>
+      <c r="K141" s="51">
+        <v>43.668709800000002</v>
+      </c>
+      <c r="L141" s="51">
+        <v>-79.394137900000004</v>
+      </c>
+      <c r="M141" s="51" t="s">
+        <v>41</v>
+      </c>
+      <c r="O141" s="51">
+        <v>9038</v>
+      </c>
+      <c r="P141" s="51" t="s">
         <v>658</v>
       </c>
-      <c r="C140" s="50" t="s">
-        <v>521</v>
-      </c>
-      <c r="D140" s="48" t="s">
-        <v>659</v>
-      </c>
-      <c r="F140" s="48">
-        <v>9002</v>
-      </c>
-      <c r="G140" s="48" t="s">
-        <v>661</v>
-      </c>
-      <c r="H140" s="48" t="s">
-        <v>660</v>
-      </c>
-      <c r="I140" s="48" t="s">
-        <v>662</v>
-      </c>
-      <c r="J140" s="48">
-        <v>300</v>
-      </c>
-      <c r="K140" s="48">
-        <v>43.638863999999899</v>
-      </c>
-      <c r="L140" s="48">
-        <v>-79.427385999999899</v>
-      </c>
-      <c r="M140" s="48" t="s">
-        <v>138</v>
-      </c>
-      <c r="O140" s="48">
-        <v>9096</v>
-      </c>
-      <c r="P140" s="48" t="s">
-        <v>150</v>
-      </c>
-      <c r="Q140" s="48">
-        <v>3600</v>
-      </c>
-      <c r="R140" s="48">
-        <v>43.659861999999997</v>
-      </c>
-      <c r="S140" s="48">
-        <v>-79.435443899999996</v>
-      </c>
-      <c r="AG140" s="48" t="s">
-        <v>673</v>
-      </c>
-    </row>
-    <row r="141" spans="1:33" s="48" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A141" s="48" t="s">
-        <v>682</v>
-      </c>
-      <c r="B141" s="49" t="s">
+      <c r="Q141" s="51">
+        <v>3600</v>
+      </c>
+      <c r="R141" s="51">
+        <v>43.654710000000001</v>
+      </c>
+      <c r="S141" s="51">
+        <v>-79.388576999999898</v>
+      </c>
+      <c r="AG141" s="51" t="s">
         <v>663</v>
       </c>
-      <c r="C141" s="50" t="s">
-        <v>525</v>
-      </c>
-      <c r="D141" s="48" t="s">
-        <v>138</v>
-      </c>
-      <c r="F141" s="48">
-        <v>9096</v>
-      </c>
-      <c r="G141" s="48" t="s">
-        <v>150</v>
-      </c>
-      <c r="H141" s="48" t="s">
-        <v>664</v>
-      </c>
-      <c r="I141" s="48" t="s">
-        <v>665</v>
-      </c>
-      <c r="J141" s="48">
-        <v>300</v>
-      </c>
-      <c r="K141" s="48">
-        <v>43.659861999999997</v>
-      </c>
-      <c r="L141" s="48">
-        <v>-79.435443899999996</v>
-      </c>
-      <c r="M141" s="48" t="s">
-        <v>659</v>
-      </c>
-      <c r="O141" s="48">
-        <v>9002</v>
-      </c>
-      <c r="P141" s="48" t="s">
-        <v>661</v>
-      </c>
-      <c r="Q141" s="48">
-        <v>3600</v>
-      </c>
-      <c r="R141" s="48">
-        <v>43.638863999999899</v>
-      </c>
-      <c r="S141" s="48">
-        <v>-79.427385999999899</v>
-      </c>
-      <c r="AG141" s="48" t="s">
-        <v>674</v>
-      </c>
-    </row>
-    <row r="142" spans="1:33" s="48" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A142" s="48" t="s">
-        <v>682</v>
-      </c>
-      <c r="B142" s="49" t="s">
-        <v>677</v>
-      </c>
-      <c r="C142" s="50" t="s">
-        <v>543</v>
-      </c>
-      <c r="D142" s="48" t="s">
-        <v>64</v>
-      </c>
-      <c r="F142" s="48">
-        <v>5266</v>
-      </c>
-      <c r="G142" s="48" t="s">
-        <v>417</v>
-      </c>
-      <c r="H142" s="48" t="s">
-        <v>679</v>
-      </c>
-      <c r="I142" s="48" t="s">
-        <v>675</v>
-      </c>
-      <c r="J142" s="48">
-        <v>300</v>
-      </c>
-      <c r="K142" s="48">
-        <v>43.649413799999898</v>
-      </c>
-      <c r="L142" s="48">
-        <v>-79.420862700000001</v>
-      </c>
-      <c r="M142" s="48" t="s">
-        <v>141</v>
-      </c>
-      <c r="O142" s="48">
-        <v>9098</v>
-      </c>
-      <c r="P142" s="48" t="s">
-        <v>154</v>
-      </c>
-      <c r="Q142" s="48">
-        <v>3600</v>
-      </c>
-      <c r="R142" s="48">
-        <v>43.661911099999998</v>
-      </c>
-      <c r="S142" s="48">
-        <v>-79.425572900000006</v>
-      </c>
-      <c r="AG142" s="48" t="s">
-        <v>695</v>
-      </c>
-    </row>
-    <row r="143" spans="1:33" s="48" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A143" s="48" t="s">
-        <v>682</v>
-      </c>
-      <c r="B143" s="49" t="s">
-        <v>676</v>
-      </c>
-      <c r="C143" s="50" t="s">
-        <v>543</v>
-      </c>
-      <c r="D143" s="48" t="s">
-        <v>141</v>
-      </c>
-      <c r="F143" s="48">
-        <v>9098</v>
-      </c>
-      <c r="G143" s="48" t="s">
-        <v>154</v>
-      </c>
-      <c r="H143" s="48" t="s">
-        <v>678</v>
-      </c>
-      <c r="I143" s="48" t="s">
-        <v>680</v>
-      </c>
-      <c r="J143" s="48">
-        <v>300</v>
-      </c>
-      <c r="K143" s="48">
-        <v>43.661911099999998</v>
-      </c>
-      <c r="L143" s="48">
-        <v>-79.425572900000006</v>
-      </c>
-      <c r="M143" s="48" t="s">
-        <v>64</v>
-      </c>
-      <c r="O143" s="48">
-        <v>5266</v>
-      </c>
-      <c r="P143" s="48" t="s">
-        <v>417</v>
-      </c>
-      <c r="Q143" s="48">
-        <v>3600</v>
-      </c>
-      <c r="R143" s="48">
-        <v>43.649413799999898</v>
-      </c>
-      <c r="S143" s="48">
-        <v>-79.420862700000001</v>
-      </c>
-      <c r="AG143" s="48" t="s">
-        <v>656</v>
-      </c>
+    </row>
+    <row r="142" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B142" s="19"/>
+      <c r="C142" s="20"/>
+      <c r="F142" s="1"/>
+      <c r="O142" s="1"/>
+    </row>
+    <row r="143" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="B143" s="19"/>
+      <c r="C143" s="20"/>
+      <c r="F143" s="1"/>
+      <c r="O143" s="1"/>
     </row>
     <row r="144" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A144" s="47" t="s">
-        <v>648</v>
-      </c>
-      <c r="B144" s="19" t="s">
-        <v>684</v>
-      </c>
-      <c r="C144" s="20" t="s">
-        <v>685</v>
-      </c>
-      <c r="D144" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F144" s="1">
-        <v>9038</v>
-      </c>
-      <c r="G144" s="1" t="s">
-        <v>688</v>
-      </c>
-      <c r="H144" s="1" t="s">
-        <v>689</v>
-      </c>
-      <c r="I144" s="1" t="s">
-        <v>690</v>
-      </c>
-      <c r="J144" s="1">
-        <v>300</v>
-      </c>
-      <c r="K144" s="1">
-        <v>43.654710000000001</v>
-      </c>
-      <c r="L144" s="1">
-        <v>-79.388576999999898</v>
-      </c>
-      <c r="M144" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="O144" s="1">
-        <v>5330</v>
-      </c>
-      <c r="P144" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="Q144" s="1">
-        <v>3600</v>
-      </c>
-      <c r="R144" s="1">
-        <v>43.668709800000002</v>
-      </c>
-      <c r="S144" s="1">
-        <v>-79.394137900000004</v>
-      </c>
-      <c r="AG144" s="47" t="s">
-        <v>694</v>
-      </c>
-    </row>
-    <row r="145" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A145" s="47" t="s">
-        <v>648</v>
-      </c>
-      <c r="B145" s="19" t="s">
-        <v>686</v>
-      </c>
-      <c r="C145" s="20" t="s">
-        <v>687</v>
-      </c>
-      <c r="D145" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="F145" s="1">
-        <v>5330</v>
-      </c>
-      <c r="G145" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="H145" s="1" t="s">
-        <v>691</v>
-      </c>
-      <c r="I145" s="1" t="s">
-        <v>692</v>
-      </c>
-      <c r="J145" s="1">
-        <v>300</v>
-      </c>
-      <c r="K145" s="1">
-        <v>43.668709800000002</v>
-      </c>
-      <c r="L145" s="1">
-        <v>-79.394137900000004</v>
-      </c>
-      <c r="M145" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="O145" s="1">
-        <v>9038</v>
-      </c>
-      <c r="P145" s="1" t="s">
-        <v>688</v>
-      </c>
-      <c r="Q145" s="1">
-        <v>3600</v>
-      </c>
-      <c r="R145" s="1">
-        <v>43.654710000000001</v>
-      </c>
-      <c r="S145" s="1">
-        <v>-79.388576999999898</v>
-      </c>
-      <c r="AG145" s="47" t="s">
-        <v>693</v>
-      </c>
-    </row>
-    <row r="146" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="B144" s="19"/>
+      <c r="C144" s="20"/>
+      <c r="F144" s="1"/>
+      <c r="O144" s="1"/>
+    </row>
+    <row r="145" spans="2:33" x14ac:dyDescent="0.2">
+      <c r="B145" s="19"/>
+      <c r="C145" s="20"/>
+      <c r="F145" s="1"/>
+      <c r="O145" s="1"/>
+    </row>
+    <row r="146" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B146" s="19"/>
       <c r="C146" s="20"/>
       <c r="F146" s="1"/>
       <c r="O146" s="1"/>
     </row>
-    <row r="147" spans="1:33" x14ac:dyDescent="0.2">
+    <row r="147" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B147" s="19"/>
       <c r="C147" s="20"/>
       <c r="F147" s="1"/>
       <c r="O147" s="1"/>
-      <c r="AG147" s="51"/>
-    </row>
-    <row r="148" spans="1:33" x14ac:dyDescent="0.2">
+    </row>
+    <row r="148" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B148" s="19"/>
       <c r="C148" s="20"/>
       <c r="F148" s="1"/>
       <c r="O148" s="1"/>
-    </row>
-    <row r="149" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="AG148" s="43"/>
+    </row>
+    <row r="149" spans="2:33" x14ac:dyDescent="0.2">
       <c r="B149" s="19"/>
       <c r="C149" s="20"/>
       <c r="F149" s="1"/>
       <c r="O149" s="1"/>
     </row>
-    <row r="150" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="B150" s="19"/>
-      <c r="C150" s="20"/>
-      <c r="F150" s="1"/>
-      <c r="O150" s="1"/>
-    </row>
-    <row r="151" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="B151" s="19"/>
-      <c r="C151" s="20"/>
-      <c r="F151" s="1"/>
-      <c r="O151" s="1"/>
-    </row>
-    <row r="152" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="B152" s="19"/>
-      <c r="C152" s="20"/>
-      <c r="F152" s="1"/>
-      <c r="O152" s="1"/>
-    </row>
-    <row r="153" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="B153" s="19"/>
-      <c r="C153" s="20"/>
-      <c r="F153" s="1"/>
-      <c r="O153" s="1"/>
-    </row>
-    <row r="154" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="B154" s="19"/>
-      <c r="C154" s="20"/>
-      <c r="F154" s="1"/>
-      <c r="O154" s="1"/>
-    </row>
-    <row r="155" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="B155" s="19"/>
-      <c r="C155" s="20"/>
-      <c r="F155" s="1"/>
-      <c r="O155" s="1"/>
-    </row>
-    <row r="156" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="B156" s="19"/>
-      <c r="C156" s="20"/>
-      <c r="F156" s="1"/>
-      <c r="O156" s="1"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A2:AF146" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A100:AF143">
-      <sortCondition ref="A2:A143"/>
+  <autoFilter ref="A2:AF142" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <filterColumn colId="0">
+      <customFilters>
+        <customFilter operator="notEqual" val=" "/>
+      </customFilters>
+    </filterColumn>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A100:AF139">
+      <sortCondition ref="A2:A139"/>
     </sortState>
   </autoFilter>
   <mergeCells count="6">
@@ -10444,14 +10210,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="62" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="60" t="s">
+      <c r="B2" s="63"/>
+      <c r="C2" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="61"/>
+      <c r="D2" s="65"/>
       <c r="E2" s="21" t="s">
         <v>57</v>
       </c>
@@ -11661,10 +11427,10 @@
     </row>
     <row r="62" spans="1:11" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="45" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B62" s="45" t="s">
-        <v>646</v>
+        <v>640</v>
       </c>
       <c r="C62" s="45">
         <v>9312</v>

</xml_diff>

<commit_message>
#234 another update with BT detector at Highpark
Bathurst and Avenue Rd  added
</commit_message>
<xml_diff>
--- a/bluetooth/update/Bliptrack TT Routes - 2020-09-08.xlsx
+++ b/bluetooth/update/Bliptrack TT Routes - 2020-09-08.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mohan\Documents\GitHub\bdit_data-sources\bluetooth\update\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A24DBF-69C2-46F7-B89A-6B6B790F302F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B882AA4-703F-438A-BBEA-CE6E10157E8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Locations!$A$3:$F$62</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Reports!$A$2:$AF$142</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Reports!$A$2:$AF$148</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -35,7 +35,7 @@
     <author>Mohanraj Adhikari</author>
   </authors>
   <commentList>
-    <comment ref="K124" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="K123" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -98,7 +98,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1295" uniqueCount="692">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1374" uniqueCount="720">
   <si>
     <t>Start point</t>
   </si>
@@ -1882,18 +1882,6 @@
     <t>5414_1, 5414_2</t>
   </si>
   <si>
-    <t>DT3_Queens-SB_Hoskin-to-College</t>
-  </si>
-  <si>
-    <t>Queens SB</t>
-  </si>
-  <si>
-    <t>HB_QP+CO_UN</t>
-  </si>
-  <si>
-    <t>5612_1, 5612_2, 5414_1, 5414_2</t>
-  </si>
-  <si>
     <t>9097_1, 9097_2</t>
   </si>
   <si>
@@ -1918,12 +1906,6 @@
     <t>5414_1, 5414_2, 9097_1, 9097_2</t>
   </si>
   <si>
-    <t>DT3_Queens-SB_Bloor-to-Hoskin</t>
-  </si>
-  <si>
-    <t>DT3_Queens-NB_Wellesley-to-Bloor</t>
-  </si>
-  <si>
     <t>WS_QP+BD_AV</t>
   </si>
   <si>
@@ -2068,12 +2050,6 @@
     <t>University NB</t>
   </si>
   <si>
-    <t>DT3_Avenue-SB_Bloor-to-Dundas</t>
-  </si>
-  <si>
-    <t>University SB</t>
-  </si>
-  <si>
     <t>9038_1, 9038_2</t>
   </si>
   <si>
@@ -2174,6 +2150,114 @@
   </si>
   <si>
     <t>DU_DF active in JJ table  but last data received in aggr_5 min table was on 2020-02-07</t>
+  </si>
+  <si>
+    <t>DT3_Bloor-WB_Bathurst-to-Dufferin</t>
+  </si>
+  <si>
+    <t>9092_1, 9092_2, 9096_1, 9096_2</t>
+  </si>
+  <si>
+    <t>DT3_Bloor-EB_Dufferin-to-Bathurst</t>
+  </si>
+  <si>
+    <t>BD_BA+BD_DF</t>
+  </si>
+  <si>
+    <t>BD_DF+BD_BA</t>
+  </si>
+  <si>
+    <t>9096_1, 9096_2, 9092_1, 9092_2</t>
+  </si>
+  <si>
+    <t>BD_BA active in jj table. Last data pulled for this detector in aggr_5min table was 2020-07-30</t>
+  </si>
+  <si>
+    <t>DT3_Bloor-EB_Bathurst-to-Avenue</t>
+  </si>
+  <si>
+    <t>BD_BA+BD_AV</t>
+  </si>
+  <si>
+    <t>9092_1, 9092_2, 5330_1, 5330_2</t>
+  </si>
+  <si>
+    <t>BD_AV+BD_BA</t>
+  </si>
+  <si>
+    <t>5330_1, 5330_2,  9092_1, 9092_2</t>
+  </si>
+  <si>
+    <t>DT3_Bloor-WB_Avenue-to-Bathurst</t>
+  </si>
+  <si>
+    <t>DT3_Queenspark-SB_Bloor-to-Dundas</t>
+  </si>
+  <si>
+    <t>DT3_Queenspark-SB_Bloor-to-Hoskin</t>
+  </si>
+  <si>
+    <t>DT3_Queenspark-NB_Wellesley-to-Bloor</t>
+  </si>
+  <si>
+    <t>Queenspark NB</t>
+  </si>
+  <si>
+    <t>Queenspark SB</t>
+  </si>
+  <si>
+    <t>CO_SP active in as per JJ active detector list. No data exists in aggr_5min table</t>
+  </si>
+  <si>
+    <t>HB_SP active in as per JJ active detector list. No data exists in aggr_5min table</t>
+  </si>
+  <si>
+    <t>HB_BA active in JJ list of active detectors. No data exists in aggr_5min table</t>
+  </si>
+  <si>
+    <t>DT3_Bathurst-SB_Harbord-to-Queen</t>
+  </si>
+  <si>
+    <t>HB_BA+QU_BA</t>
+  </si>
+  <si>
+    <t>9090_1, 9090_2, 9036_1, 9036_2</t>
+  </si>
+  <si>
+    <t>QU_BA</t>
+  </si>
+  <si>
+    <t>9036_1, 9036_2</t>
+  </si>
+  <si>
+    <t>DT3_Bathurst-NB_Queen-to-Harbord</t>
+  </si>
+  <si>
+    <t>QU_BA+HB_BA</t>
+  </si>
+  <si>
+    <t>9036_1, 9036_2, 9090_1, 9090_2</t>
+  </si>
+  <si>
+    <t>QU_BA is active in jj list of active detectors. Data exists in aggr_5min table latest 2020-09-17</t>
+  </si>
+  <si>
+    <t>DU_UN+WS_QP</t>
+  </si>
+  <si>
+    <t>DT3_University-NB_Dundas-to-Wellesley</t>
+  </si>
+  <si>
+    <t>9038_1, 9038_2, 9097_1, 9097_2</t>
+  </si>
+  <si>
+    <t>DT3_Queenspark-SB_Hoskin-to-Dundas</t>
+  </si>
+  <si>
+    <t>HB_QP+DU_UN</t>
+  </si>
+  <si>
+    <t>5612_1, 5612_2, 9038_1, 9038_2</t>
   </si>
 </sst>
 </file>
@@ -2273,7 +2357,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2313,12 +2397,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
@@ -2493,7 +2571,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -2546,7 +2624,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2555,21 +2632,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="12" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2884,13 +2961,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:AG149"/>
+  <dimension ref="A1:AG148"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="5" ySplit="99" topLeftCell="AF100" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A100" sqref="A100"/>
-      <selection pane="bottomRight" activeCell="A140" sqref="A140:XFD141"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="S3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="B143" sqref="B143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -2928,53 +3005,53 @@
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>644</v>
-      </c>
-      <c r="B1" s="56" t="s">
+        <v>638</v>
+      </c>
+      <c r="B1" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="56"/>
-      <c r="D1" s="57" t="s">
+      <c r="C1" s="55"/>
+      <c r="D1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="58" t="s">
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="58"/>
-      <c r="O1" s="58"/>
-      <c r="P1" s="58"/>
-      <c r="Q1" s="58"/>
-      <c r="R1" s="58"/>
-      <c r="S1" s="58"/>
-      <c r="T1" s="60" t="s">
+      <c r="N1" s="57"/>
+      <c r="O1" s="57"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="57"/>
+      <c r="R1" s="57"/>
+      <c r="S1" s="57"/>
+      <c r="T1" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="U1" s="60"/>
-      <c r="V1" s="60"/>
-      <c r="W1" s="61" t="s">
+      <c r="U1" s="59"/>
+      <c r="V1" s="59"/>
+      <c r="W1" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="X1" s="61"/>
-      <c r="Y1" s="61"/>
-      <c r="Z1" s="59" t="s">
+      <c r="X1" s="60"/>
+      <c r="Y1" s="60"/>
+      <c r="Z1" s="58" t="s">
         <v>18</v>
       </c>
-      <c r="AA1" s="59"/>
-      <c r="AB1" s="59"/>
-      <c r="AC1" s="59"/>
-      <c r="AD1" s="59"/>
-      <c r="AE1" s="59"/>
-      <c r="AF1" s="59"/>
+      <c r="AA1" s="58"/>
+      <c r="AB1" s="58"/>
+      <c r="AC1" s="58"/>
+      <c r="AD1" s="58"/>
+      <c r="AE1" s="58"/>
+      <c r="AF1" s="58"/>
       <c r="AG1" s="1" t="s">
-        <v>643</v>
+        <v>637</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.2">
@@ -7922,116 +7999,116 @@
         <v>-79.452438400000005</v>
       </c>
     </row>
-    <row r="100" spans="1:33" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="51" t="s">
-        <v>652</v>
-      </c>
-      <c r="B100" s="52" t="s">
+    <row r="100" spans="1:33" s="50" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="50" t="s">
+        <v>646</v>
+      </c>
+      <c r="B100" s="51" t="s">
+        <v>662</v>
+      </c>
+      <c r="C100" s="52" t="s">
+        <v>287</v>
+      </c>
+      <c r="D100" s="50" t="s">
+        <v>657</v>
+      </c>
+      <c r="F100" s="50">
+        <v>5819</v>
+      </c>
+      <c r="G100" s="50" t="s">
+        <v>660</v>
+      </c>
+      <c r="H100" s="50" t="s">
+        <v>663</v>
+      </c>
+      <c r="I100" s="50" t="s">
+        <v>664</v>
+      </c>
+      <c r="J100" s="50">
+        <v>300</v>
+      </c>
+      <c r="K100" s="50">
+        <v>43.653686999999998</v>
+      </c>
+      <c r="L100" s="50">
+        <v>-79.465096000000003</v>
+      </c>
+      <c r="M100" s="50" t="s">
+        <v>515</v>
+      </c>
+      <c r="O100" s="50">
+        <v>9312</v>
+      </c>
+      <c r="P100" s="50" t="s">
+        <v>516</v>
+      </c>
+      <c r="Q100" s="50">
+        <v>3600</v>
+      </c>
+      <c r="R100" s="50">
+        <v>43.651156999999898</v>
+      </c>
+      <c r="S100" s="50">
+        <v>-79.476039999999898</v>
+      </c>
+      <c r="AG100" s="50" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="101" spans="1:33" s="50" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="50" t="s">
+        <v>646</v>
+      </c>
+      <c r="B101" s="51" t="s">
+        <v>661</v>
+      </c>
+      <c r="C101" s="52" t="s">
+        <v>146</v>
+      </c>
+      <c r="D101" s="50" t="s">
+        <v>515</v>
+      </c>
+      <c r="F101" s="50">
+        <v>9312</v>
+      </c>
+      <c r="G101" s="50" t="s">
+        <v>516</v>
+      </c>
+      <c r="H101" s="50" t="s">
+        <v>658</v>
+      </c>
+      <c r="I101" s="50" t="s">
+        <v>659</v>
+      </c>
+      <c r="J101" s="50">
+        <v>300</v>
+      </c>
+      <c r="K101" s="50">
+        <v>43.651156999999898</v>
+      </c>
+      <c r="L101" s="50">
+        <v>-79.476039999999898</v>
+      </c>
+      <c r="M101" s="50" t="s">
+        <v>657</v>
+      </c>
+      <c r="O101" s="50">
+        <v>5819</v>
+      </c>
+      <c r="P101" s="50" t="s">
         <v>670</v>
       </c>
-      <c r="C100" s="53" t="s">
-        <v>287</v>
-      </c>
-      <c r="D100" s="51" t="s">
-        <v>665</v>
-      </c>
-      <c r="F100" s="51">
-        <v>5819</v>
-      </c>
-      <c r="G100" s="51" t="s">
-        <v>668</v>
-      </c>
-      <c r="H100" s="51" t="s">
-        <v>671</v>
-      </c>
-      <c r="I100" s="51" t="s">
-        <v>672</v>
-      </c>
-      <c r="J100" s="51">
-        <v>300</v>
-      </c>
-      <c r="K100" s="51">
+      <c r="Q101" s="50">
+        <v>3600</v>
+      </c>
+      <c r="R101" s="50">
         <v>43.653686999999998</v>
       </c>
-      <c r="L100" s="51">
+      <c r="S101" s="50">
         <v>-79.465096000000003</v>
       </c>
-      <c r="M100" s="51" t="s">
-        <v>515</v>
-      </c>
-      <c r="O100" s="51">
-        <v>9312</v>
-      </c>
-      <c r="P100" s="51" t="s">
-        <v>516</v>
-      </c>
-      <c r="Q100" s="51">
-        <v>3600</v>
-      </c>
-      <c r="R100" s="51">
-        <v>43.651156999999898</v>
-      </c>
-      <c r="S100" s="51">
-        <v>-79.476039999999898</v>
-      </c>
-      <c r="AG100" s="51" t="s">
+      <c r="AG101" s="50" t="s">
         <v>680</v>
-      </c>
-    </row>
-    <row r="101" spans="1:33" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="51" t="s">
-        <v>652</v>
-      </c>
-      <c r="B101" s="52" t="s">
-        <v>669</v>
-      </c>
-      <c r="C101" s="53" t="s">
-        <v>146</v>
-      </c>
-      <c r="D101" s="51" t="s">
-        <v>515</v>
-      </c>
-      <c r="F101" s="51">
-        <v>9312</v>
-      </c>
-      <c r="G101" s="51" t="s">
-        <v>516</v>
-      </c>
-      <c r="H101" s="51" t="s">
-        <v>666</v>
-      </c>
-      <c r="I101" s="51" t="s">
-        <v>667</v>
-      </c>
-      <c r="J101" s="51">
-        <v>300</v>
-      </c>
-      <c r="K101" s="51">
-        <v>43.651156999999898</v>
-      </c>
-      <c r="L101" s="51">
-        <v>-79.476039999999898</v>
-      </c>
-      <c r="M101" s="51" t="s">
-        <v>665</v>
-      </c>
-      <c r="O101" s="51">
-        <v>5819</v>
-      </c>
-      <c r="P101" s="51" t="s">
-        <v>678</v>
-      </c>
-      <c r="Q101" s="51">
-        <v>3600</v>
-      </c>
-      <c r="R101" s="51">
-        <v>43.653686999999998</v>
-      </c>
-      <c r="S101" s="51">
-        <v>-79.465096000000003</v>
-      </c>
-      <c r="AG101" s="51" t="s">
-        <v>688</v>
       </c>
     </row>
     <row r="102" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
@@ -8054,7 +8131,7 @@
         <v>519</v>
       </c>
       <c r="I102" s="1" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="J102" s="1">
         <v>300</v>
@@ -8072,7 +8149,7 @@
         <v>5412</v>
       </c>
       <c r="P102" s="1" t="s">
-        <v>626</v>
+        <v>620</v>
       </c>
       <c r="Q102" s="1">
         <v>3600</v>
@@ -8098,7 +8175,7 @@
         <v>5412</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>626</v>
+        <v>620</v>
       </c>
       <c r="H103" s="1" t="s">
         <v>522</v>
@@ -8148,7 +8225,7 @@
         <v>5412</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>626</v>
+        <v>620</v>
       </c>
       <c r="H104" s="1" t="s">
         <v>523</v>
@@ -8204,7 +8281,7 @@
         <v>524</v>
       </c>
       <c r="I105" s="1" t="s">
-        <v>635</v>
+        <v>629</v>
       </c>
       <c r="J105" s="1">
         <v>300</v>
@@ -8222,7 +8299,7 @@
         <v>5412</v>
       </c>
       <c r="P105" s="1" t="s">
-        <v>626</v>
+        <v>620</v>
       </c>
       <c r="Q105" s="1">
         <v>3600</v>
@@ -8248,7 +8325,7 @@
         <v>5412</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>626</v>
+        <v>620</v>
       </c>
       <c r="H106" s="1" t="s">
         <v>531</v>
@@ -8272,7 +8349,7 @@
         <v>5272</v>
       </c>
       <c r="P106" s="1" t="s">
-        <v>627</v>
+        <v>621</v>
       </c>
       <c r="Q106" s="1">
         <v>3600</v>
@@ -8304,7 +8381,7 @@
         <v>535</v>
       </c>
       <c r="I107" s="1" t="s">
-        <v>636</v>
+        <v>630</v>
       </c>
       <c r="J107" s="1">
         <v>300</v>
@@ -8354,7 +8431,7 @@
         <v>538</v>
       </c>
       <c r="I108" s="1" t="s">
-        <v>637</v>
+        <v>631</v>
       </c>
       <c r="J108" s="1">
         <v>300</v>
@@ -8404,7 +8481,7 @@
         <v>542</v>
       </c>
       <c r="I109" s="1" t="s">
-        <v>638</v>
+        <v>632</v>
       </c>
       <c r="J109" s="1">
         <v>300</v>
@@ -8434,307 +8511,331 @@
         <v>-79.422612200000003</v>
       </c>
     </row>
-    <row r="110" spans="1:33" s="43" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B110" s="41" t="s">
+    <row r="110" spans="1:33" s="42" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B110" s="40" t="s">
         <v>543</v>
       </c>
-      <c r="C110" s="42" t="s">
+      <c r="C110" s="41" t="s">
         <v>544</v>
       </c>
-      <c r="D110" s="43" t="s">
+      <c r="D110" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="F110" s="43">
+      <c r="F110" s="42">
         <v>5268</v>
       </c>
-      <c r="G110" s="43" t="s">
+      <c r="G110" s="42" t="s">
         <v>147</v>
       </c>
-      <c r="H110" s="43" t="s">
+      <c r="H110" s="42" t="s">
         <v>545</v>
       </c>
-      <c r="I110" s="43" t="s">
+      <c r="I110" s="42" t="s">
         <v>546</v>
       </c>
-      <c r="J110" s="43">
-        <v>300</v>
-      </c>
-      <c r="K110" s="43">
+      <c r="J110" s="42">
+        <v>300</v>
+      </c>
+      <c r="K110" s="42">
         <v>43.6565569999999</v>
       </c>
-      <c r="L110" s="43">
+      <c r="L110" s="42">
         <v>-79.407966000000002</v>
       </c>
-      <c r="M110" s="43" t="s">
+      <c r="M110" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="O110" s="43">
+      <c r="O110" s="42">
         <v>9090</v>
       </c>
-      <c r="P110" s="43" t="s">
+      <c r="P110" s="42" t="s">
         <v>550</v>
       </c>
-      <c r="Q110" s="43">
-        <v>3600</v>
-      </c>
-      <c r="R110" s="43">
+      <c r="Q110" s="42">
+        <v>3600</v>
+      </c>
+      <c r="R110" s="42">
         <v>43.661569499999899</v>
       </c>
-      <c r="S110" s="43">
+      <c r="S110" s="42">
         <v>-79.4097376</v>
       </c>
     </row>
-    <row r="111" spans="1:33" s="43" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B111" s="41" t="s">
+    <row r="111" spans="1:33" s="42" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B111" s="40" t="s">
         <v>551</v>
       </c>
-      <c r="C111" s="42" t="s">
+      <c r="C111" s="41" t="s">
         <v>552</v>
       </c>
-      <c r="D111" s="43" t="s">
+      <c r="D111" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="F111" s="43">
+      <c r="F111" s="42">
         <v>9090</v>
       </c>
-      <c r="G111" s="43" t="s">
+      <c r="G111" s="42" t="s">
         <v>550</v>
       </c>
-      <c r="H111" s="43" t="s">
+      <c r="H111" s="42" t="s">
         <v>553</v>
       </c>
-      <c r="I111" s="43" t="s">
+      <c r="I111" s="42" t="s">
         <v>554</v>
       </c>
-      <c r="J111" s="43">
-        <v>300</v>
-      </c>
-      <c r="K111" s="43">
+      <c r="J111" s="42">
+        <v>300</v>
+      </c>
+      <c r="K111" s="42">
         <v>43.661569499999899</v>
       </c>
-      <c r="L111" s="43">
+      <c r="L111" s="42">
         <v>-79.4097376</v>
       </c>
-      <c r="M111" s="43" t="s">
+      <c r="M111" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="O111" s="43">
+      <c r="O111" s="42">
         <v>5268</v>
       </c>
-      <c r="P111" s="43" t="s">
+      <c r="P111" s="42" t="s">
         <v>147</v>
       </c>
-      <c r="Q111" s="43">
-        <v>3600</v>
-      </c>
-      <c r="R111" s="43">
+      <c r="Q111" s="42">
+        <v>3600</v>
+      </c>
+      <c r="R111" s="42">
         <v>43.6565569999999</v>
       </c>
-      <c r="S111" s="43">
+      <c r="S111" s="42">
         <v>-79.407966000000002</v>
       </c>
     </row>
-    <row r="112" spans="1:33" s="43" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B112" s="41" t="s">
+    <row r="112" spans="1:33" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A112" s="47" t="s">
+        <v>647</v>
+      </c>
+      <c r="B112" s="48" t="s">
         <v>555</v>
       </c>
-      <c r="C112" s="42" t="s">
+      <c r="C112" s="49" t="s">
         <v>544</v>
       </c>
-      <c r="D112" s="43" t="s">
+      <c r="D112" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="F112" s="43">
+      <c r="F112" s="47">
         <v>9090</v>
       </c>
-      <c r="G112" s="43" t="s">
+      <c r="G112" s="47" t="s">
         <v>550</v>
       </c>
-      <c r="H112" s="43" t="s">
+      <c r="H112" s="47" t="s">
         <v>556</v>
       </c>
-      <c r="I112" s="43" t="s">
+      <c r="I112" s="47" t="s">
         <v>557</v>
       </c>
-      <c r="J112" s="43">
-        <v>300</v>
-      </c>
-      <c r="K112" s="43">
+      <c r="J112" s="47">
+        <v>300</v>
+      </c>
+      <c r="K112" s="47">
         <v>43.661569499999899</v>
       </c>
-      <c r="L112" s="43">
+      <c r="L112" s="47">
         <v>-79.4097376</v>
       </c>
-      <c r="M112" s="43" t="s">
+      <c r="M112" s="47" t="s">
         <v>136</v>
       </c>
-      <c r="O112" s="43">
+      <c r="O112" s="47">
         <v>9092</v>
       </c>
-      <c r="P112" s="43" t="s">
+      <c r="P112" s="47" t="s">
         <v>558</v>
       </c>
-      <c r="Q112" s="43">
-        <v>3600</v>
-      </c>
-      <c r="R112" s="43">
+      <c r="Q112" s="47">
+        <v>3600</v>
+      </c>
+      <c r="R112" s="47">
         <v>43.665108699999898</v>
       </c>
-      <c r="S112" s="43">
+      <c r="S112" s="47">
         <v>-79.411196700000005</v>
       </c>
-    </row>
-    <row r="113" spans="2:19" s="43" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B113" s="41" t="s">
+      <c r="AG112" s="47" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="113" spans="1:33" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A113" s="47" t="s">
+        <v>647</v>
+      </c>
+      <c r="B113" s="48" t="s">
         <v>559</v>
       </c>
-      <c r="C113" s="42" t="s">
+      <c r="C113" s="49" t="s">
         <v>552</v>
       </c>
-      <c r="D113" s="43" t="s">
+      <c r="D113" s="47" t="s">
         <v>136</v>
       </c>
-      <c r="F113" s="43">
+      <c r="F113" s="47">
         <v>9092</v>
       </c>
-      <c r="G113" s="43" t="s">
+      <c r="G113" s="47" t="s">
         <v>558</v>
       </c>
-      <c r="H113" s="43" t="s">
+      <c r="H113" s="47" t="s">
         <v>560</v>
       </c>
-      <c r="I113" s="43" t="s">
-        <v>612</v>
-      </c>
-      <c r="J113" s="43">
-        <v>300</v>
-      </c>
-      <c r="K113" s="43">
+      <c r="I113" s="47" t="s">
+        <v>606</v>
+      </c>
+      <c r="J113" s="47">
+        <v>300</v>
+      </c>
+      <c r="K113" s="47">
         <v>43.665108699999898</v>
       </c>
-      <c r="L113" s="43">
+      <c r="L113" s="47">
         <v>-79.411196700000005</v>
       </c>
-      <c r="M113" s="43" t="s">
+      <c r="M113" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="O113" s="43">
+      <c r="O113" s="47">
         <v>9090</v>
       </c>
-      <c r="P113" s="43" t="s">
+      <c r="P113" s="47" t="s">
         <v>550</v>
       </c>
-      <c r="Q113" s="43">
-        <v>3600</v>
-      </c>
-      <c r="R113" s="43">
+      <c r="Q113" s="47">
+        <v>3600</v>
+      </c>
+      <c r="R113" s="47">
         <v>43.661569499999899</v>
       </c>
-      <c r="S113" s="43">
+      <c r="S113" s="47">
         <v>-79.4097376</v>
       </c>
-    </row>
-    <row r="114" spans="2:19" s="43" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B114" s="41" t="s">
+      <c r="AG113" s="47" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="114" spans="1:33" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A114" s="47" t="s">
+        <v>647</v>
+      </c>
+      <c r="B114" s="48" t="s">
         <v>569</v>
       </c>
-      <c r="C114" s="42" t="s">
+      <c r="C114" s="49" t="s">
         <v>561</v>
       </c>
-      <c r="D114" s="43" t="s">
+      <c r="D114" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="F114" s="43">
+      <c r="F114" s="47">
         <v>9093</v>
       </c>
-      <c r="G114" s="43" t="s">
+      <c r="G114" s="47" t="s">
         <v>562</v>
       </c>
-      <c r="H114" s="43" t="s">
+      <c r="H114" s="47" t="s">
         <v>563</v>
       </c>
-      <c r="I114" s="43" t="s">
+      <c r="I114" s="47" t="s">
         <v>564</v>
       </c>
-      <c r="J114" s="43">
-        <v>300</v>
-      </c>
-      <c r="K114" s="43">
+      <c r="J114" s="47">
+        <v>300</v>
+      </c>
+      <c r="K114" s="47">
         <v>43.6579215</v>
       </c>
-      <c r="L114" s="43">
+      <c r="L114" s="47">
         <v>-79.400038699999897</v>
       </c>
-      <c r="M114" s="43" t="s">
+      <c r="M114" s="47" t="s">
         <v>72</v>
       </c>
-      <c r="O114" s="43">
+      <c r="O114" s="47">
         <v>9100</v>
       </c>
-      <c r="P114" s="43" t="s">
+      <c r="P114" s="47" t="s">
         <v>566</v>
       </c>
-      <c r="Q114" s="43">
-        <v>3600</v>
-      </c>
-      <c r="R114" s="43">
+      <c r="Q114" s="47">
+        <v>3600</v>
+      </c>
+      <c r="R114" s="47">
         <v>43.6630597999999</v>
       </c>
-      <c r="S114" s="43">
+      <c r="S114" s="47">
         <v>-79.402141599999894</v>
       </c>
-    </row>
-    <row r="115" spans="2:19" s="43" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B115" s="41" t="s">
+      <c r="AG114" s="47" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="115" spans="1:33" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A115" s="47" t="s">
+        <v>647</v>
+      </c>
+      <c r="B115" s="48" t="s">
         <v>570</v>
       </c>
-      <c r="C115" s="42" t="s">
+      <c r="C115" s="49" t="s">
         <v>565</v>
       </c>
-      <c r="D115" s="43" t="s">
+      <c r="D115" s="47" t="s">
         <v>72</v>
       </c>
-      <c r="F115" s="43">
+      <c r="F115" s="47">
         <v>9100</v>
       </c>
-      <c r="G115" s="43" t="s">
+      <c r="G115" s="47" t="s">
         <v>566</v>
       </c>
-      <c r="H115" s="43" t="s">
+      <c r="H115" s="47" t="s">
         <v>568</v>
       </c>
-      <c r="I115" s="43" t="s">
+      <c r="I115" s="47" t="s">
         <v>567</v>
       </c>
-      <c r="J115" s="43">
-        <v>300</v>
-      </c>
-      <c r="K115" s="43">
+      <c r="J115" s="47">
+        <v>300</v>
+      </c>
+      <c r="K115" s="47">
         <v>43.6630597999999</v>
       </c>
-      <c r="L115" s="43">
+      <c r="L115" s="47">
         <v>-79.402141599999894</v>
       </c>
-      <c r="M115" s="43" t="s">
+      <c r="M115" s="47" t="s">
         <v>60</v>
       </c>
-      <c r="O115" s="43">
+      <c r="O115" s="47">
         <v>9093</v>
       </c>
-      <c r="P115" s="43" t="s">
+      <c r="P115" s="47" t="s">
         <v>562</v>
       </c>
-      <c r="Q115" s="43">
-        <v>3600</v>
-      </c>
-      <c r="R115" s="43">
+      <c r="Q115" s="47">
+        <v>3600</v>
+      </c>
+      <c r="R115" s="47">
         <v>43.6579215</v>
       </c>
-      <c r="S115" s="43">
+      <c r="S115" s="47">
         <v>-79.400038699999897</v>
       </c>
-    </row>
-    <row r="116" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
+      <c r="AG115" s="47" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="116" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="B116" s="19" t="s">
         <v>571</v>
       </c>
@@ -8784,7 +8885,7 @@
         <v>-79.403815300000005</v>
       </c>
     </row>
-    <row r="117" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="B117" s="19" t="s">
         <v>573</v>
       </c>
@@ -8834,7 +8935,7 @@
         <v>-79.402141599999894</v>
       </c>
     </row>
-    <row r="118" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="B118" s="19" t="s">
         <v>580</v>
       </c>
@@ -8844,25 +8945,25 @@
       <c r="D118" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="F118" s="43">
+      <c r="F118" s="42">
         <v>9090</v>
       </c>
-      <c r="G118" s="43" t="s">
+      <c r="G118" s="42" t="s">
         <v>550</v>
       </c>
-      <c r="H118" s="43" t="s">
+      <c r="H118" s="42" t="s">
         <v>578</v>
       </c>
-      <c r="I118" s="43" t="s">
+      <c r="I118" s="42" t="s">
         <v>584</v>
       </c>
-      <c r="J118" s="43">
-        <v>300</v>
-      </c>
-      <c r="K118" s="43">
+      <c r="J118" s="42">
+        <v>300</v>
+      </c>
+      <c r="K118" s="42">
         <v>43.661569499999899</v>
       </c>
-      <c r="L118" s="43">
+      <c r="L118" s="42">
         <v>-79.4097376</v>
       </c>
       <c r="M118" s="1" t="s">
@@ -8884,7 +8985,7 @@
         <v>-79.402141599999894</v>
       </c>
     </row>
-    <row r="119" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="B119" s="19" t="s">
         <v>579</v>
       </c>
@@ -8900,7 +9001,7 @@
       <c r="G119" s="1" t="s">
         <v>566</v>
       </c>
-      <c r="H119" s="43" t="s">
+      <c r="H119" s="42" t="s">
         <v>582</v>
       </c>
       <c r="I119" s="1" t="s">
@@ -8918,23 +9019,23 @@
       <c r="M119" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="O119" s="43">
+      <c r="O119" s="42">
         <v>9090</v>
       </c>
-      <c r="P119" s="43" t="s">
+      <c r="P119" s="42" t="s">
         <v>550</v>
       </c>
       <c r="Q119" s="1">
         <v>3600</v>
       </c>
-      <c r="R119" s="43">
+      <c r="R119" s="42">
         <v>43.661569499999899</v>
       </c>
-      <c r="S119" s="43">
+      <c r="S119" s="42">
         <v>-79.4097376</v>
       </c>
     </row>
-    <row r="120" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="B120" s="19" t="s">
         <v>585</v>
       </c>
@@ -8950,7 +9051,7 @@
       <c r="G120" s="1" t="s">
         <v>566</v>
       </c>
-      <c r="H120" s="43" t="s">
+      <c r="H120" s="42" t="s">
         <v>588</v>
       </c>
       <c r="I120" s="1" t="s">
@@ -8984,12 +9085,12 @@
         <v>-79.393966199999895</v>
       </c>
     </row>
-    <row r="121" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="B121" s="19" t="s">
         <v>587</v>
       </c>
       <c r="C121" s="20" t="s">
-        <v>641</v>
+        <v>635</v>
       </c>
       <c r="D121" s="1" t="s">
         <v>84</v>
@@ -9034,9 +9135,9 @@
         <v>-79.402141599999894</v>
       </c>
     </row>
-    <row r="122" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="B122" s="1" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="C122" s="1" t="s">
         <v>592</v>
@@ -9051,10 +9152,10 @@
         <v>593</v>
       </c>
       <c r="H122" s="1" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="I122" s="1" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="J122" s="1">
         <v>300</v>
@@ -9072,7 +9173,7 @@
         <v>9097</v>
       </c>
       <c r="P122" s="1" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="Q122" s="1">
         <v>3600</v>
@@ -9084,215 +9185,220 @@
         <v>-79.390618799999899</v>
       </c>
     </row>
-    <row r="123" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B123" s="1" t="s">
+    <row r="123" spans="1:33" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="47" t="s">
+        <v>647</v>
+      </c>
+      <c r="B123" s="47" t="s">
+        <v>699</v>
+      </c>
+      <c r="C123" s="47" t="s">
+        <v>700</v>
+      </c>
+      <c r="D123" s="47" t="s">
+        <v>78</v>
+      </c>
+      <c r="F123" s="47">
+        <v>9097</v>
+      </c>
+      <c r="G123" s="47" t="s">
         <v>594</v>
       </c>
-      <c r="C123" s="1" t="s">
+      <c r="H123" s="47" t="s">
+        <v>602</v>
+      </c>
+      <c r="I123" s="47" t="s">
+        <v>603</v>
+      </c>
+      <c r="J123" s="47">
+        <v>300</v>
+      </c>
+      <c r="K123" s="47">
+        <v>43.6649689999999</v>
+      </c>
+      <c r="L123" s="47">
+        <v>-79.393966199999895</v>
+      </c>
+      <c r="M123" s="47" t="s">
+        <v>135</v>
+      </c>
+      <c r="O123" s="47">
+        <v>5330</v>
+      </c>
+      <c r="P123" s="47" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q123" s="47">
+        <v>3600</v>
+      </c>
+      <c r="R123" s="47">
+        <v>43.668709800000002</v>
+      </c>
+      <c r="S123" s="47">
+        <v>-79.394137900000004</v>
+      </c>
+    </row>
+    <row r="124" spans="1:33" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A124" s="47" t="s">
+        <v>647</v>
+      </c>
+      <c r="B124" s="48" t="s">
+        <v>698</v>
+      </c>
+      <c r="C124" s="49" t="s">
+        <v>701</v>
+      </c>
+      <c r="D124" s="47" t="s">
+        <v>135</v>
+      </c>
+      <c r="F124" s="47">
+        <v>5330</v>
+      </c>
+      <c r="G124" s="47" t="s">
+        <v>166</v>
+      </c>
+      <c r="H124" s="47" t="s">
         <v>595</v>
       </c>
-      <c r="D123" s="1" t="s">
+      <c r="I124" s="47" t="s">
+        <v>596</v>
+      </c>
+      <c r="J124" s="47">
+        <v>300</v>
+      </c>
+      <c r="K124" s="47">
+        <v>43.668709800000002</v>
+      </c>
+      <c r="L124" s="47">
+        <v>-79.394137900000004</v>
+      </c>
+      <c r="M124" s="47" t="s">
         <v>84</v>
       </c>
-      <c r="F123" s="1">
+      <c r="O124" s="47">
         <v>5612</v>
       </c>
-      <c r="G123" s="1" t="s">
+      <c r="P124" s="47" t="s">
         <v>586</v>
       </c>
-      <c r="H123" s="1" t="s">
-        <v>596</v>
-      </c>
-      <c r="I123" s="1" t="s">
+      <c r="Q124" s="47">
+        <v>3600</v>
+      </c>
+      <c r="R124" s="47">
+        <v>43.6649689999999</v>
+      </c>
+      <c r="S124" s="47">
+        <v>-79.393966199999895</v>
+      </c>
+    </row>
+    <row r="125" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B125" s="19" t="s">
         <v>597</v>
       </c>
-      <c r="J123" s="1">
-        <v>300</v>
-      </c>
-      <c r="K123" s="1">
+      <c r="C125" s="20" t="s">
+        <v>598</v>
+      </c>
+      <c r="D125" s="42" t="s">
+        <v>78</v>
+      </c>
+      <c r="E125" s="42"/>
+      <c r="F125" s="42">
+        <v>9097</v>
+      </c>
+      <c r="G125" s="42" t="s">
+        <v>594</v>
+      </c>
+      <c r="H125" s="42" t="s">
+        <v>604</v>
+      </c>
+      <c r="I125" s="42" t="s">
+        <v>605</v>
+      </c>
+      <c r="J125" s="42">
+        <v>300</v>
+      </c>
+      <c r="K125" s="42">
         <v>43.6649689999999</v>
       </c>
-      <c r="L123" s="1">
+      <c r="L125" s="42">
         <v>-79.393966199999895</v>
       </c>
-      <c r="M123" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="O123" s="1">
-        <v>5414</v>
-      </c>
-      <c r="P123" s="1" t="s">
-        <v>593</v>
-      </c>
-      <c r="Q123" s="1">
-        <v>3600</v>
-      </c>
-      <c r="R123" s="1">
-        <v>43.659647999999898</v>
-      </c>
-      <c r="S123" s="1">
-        <v>-79.390716999999896</v>
-      </c>
-    </row>
-    <row r="124" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B124" s="40" t="s">
+      <c r="M125" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="O125" s="1">
+        <v>5329</v>
+      </c>
+      <c r="P125" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="Q125" s="1">
+        <v>3600</v>
+      </c>
+      <c r="R125" s="1">
+        <v>43.6649379999999</v>
+      </c>
+      <c r="S125" s="1">
+        <v>-79.3845034</v>
+      </c>
+    </row>
+    <row r="126" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B126" s="19" t="s">
         <v>607</v>
       </c>
-      <c r="C124" s="40" t="s">
-        <v>592</v>
-      </c>
-      <c r="D124" s="40" t="s">
+      <c r="C126" s="20" t="s">
+        <v>608</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F126" s="1">
+        <v>5329</v>
+      </c>
+      <c r="G126" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="H126" s="42" t="s">
+        <v>609</v>
+      </c>
+      <c r="I126" s="42" t="s">
+        <v>610</v>
+      </c>
+      <c r="J126" s="42">
+        <v>300</v>
+      </c>
+      <c r="K126" s="1">
+        <v>43.6649379999999</v>
+      </c>
+      <c r="L126" s="1">
+        <v>-79.3845034</v>
+      </c>
+      <c r="M126" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="E124" s="40"/>
-      <c r="F124" s="40">
+      <c r="N126" s="42"/>
+      <c r="O126" s="42">
         <v>9097</v>
       </c>
-      <c r="G124" s="40" t="s">
+      <c r="P126" s="42" t="s">
+        <v>594</v>
+      </c>
+      <c r="Q126" s="1">
+        <v>3600</v>
+      </c>
+      <c r="R126" s="42">
+        <v>43.6649689999999</v>
+      </c>
+      <c r="S126" s="42">
+        <v>-79.393966199999895</v>
+      </c>
+    </row>
+    <row r="127" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
+      <c r="B127" s="19" t="s">
+        <v>611</v>
+      </c>
+      <c r="C127" s="20" t="s">
         <v>598</v>
-      </c>
-      <c r="H124" s="40" t="s">
-        <v>608</v>
-      </c>
-      <c r="I124" s="40" t="s">
-        <v>609</v>
-      </c>
-      <c r="J124" s="40">
-        <v>300</v>
-      </c>
-      <c r="K124" s="40">
-        <v>43.6649689999999</v>
-      </c>
-      <c r="L124" s="40">
-        <v>-79.393966199999895</v>
-      </c>
-      <c r="M124" s="40" t="s">
-        <v>135</v>
-      </c>
-      <c r="N124" s="40"/>
-      <c r="O124" s="40">
-        <v>5330</v>
-      </c>
-      <c r="P124" s="40" t="s">
-        <v>166</v>
-      </c>
-      <c r="Q124" s="40">
-        <v>3600</v>
-      </c>
-      <c r="R124" s="40">
-        <v>43.668709800000002</v>
-      </c>
-      <c r="S124" s="40">
-        <v>-79.394137900000004</v>
-      </c>
-    </row>
-    <row r="125" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B125" s="19" t="s">
-        <v>606</v>
-      </c>
-      <c r="C125" s="20" t="s">
-        <v>595</v>
-      </c>
-      <c r="D125" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="F125" s="1">
-        <v>5330</v>
-      </c>
-      <c r="G125" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="H125" s="1" t="s">
-        <v>599</v>
-      </c>
-      <c r="I125" s="1" t="s">
-        <v>600</v>
-      </c>
-      <c r="J125" s="1">
-        <v>300</v>
-      </c>
-      <c r="K125" s="1">
-        <v>43.668709800000002</v>
-      </c>
-      <c r="L125" s="1">
-        <v>-79.394137900000004</v>
-      </c>
-      <c r="M125" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="O125" s="1">
-        <v>5612</v>
-      </c>
-      <c r="P125" s="1" t="s">
-        <v>586</v>
-      </c>
-      <c r="Q125" s="1">
-        <v>3600</v>
-      </c>
-      <c r="R125" s="1">
-        <v>43.6649689999999</v>
-      </c>
-      <c r="S125" s="1">
-        <v>-79.393966199999895</v>
-      </c>
-    </row>
-    <row r="126" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B126" s="19" t="s">
-        <v>601</v>
-      </c>
-      <c r="C126" s="20" t="s">
-        <v>602</v>
-      </c>
-      <c r="D126" s="43" t="s">
-        <v>78</v>
-      </c>
-      <c r="E126" s="43"/>
-      <c r="F126" s="43">
-        <v>9097</v>
-      </c>
-      <c r="G126" s="43" t="s">
-        <v>598</v>
-      </c>
-      <c r="H126" s="43" t="s">
-        <v>610</v>
-      </c>
-      <c r="I126" s="43" t="s">
-        <v>611</v>
-      </c>
-      <c r="J126" s="43">
-        <v>300</v>
-      </c>
-      <c r="K126" s="43">
-        <v>43.6649689999999</v>
-      </c>
-      <c r="L126" s="43">
-        <v>-79.393966199999895</v>
-      </c>
-      <c r="M126" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="O126" s="1">
-        <v>5329</v>
-      </c>
-      <c r="P126" s="1" t="s">
-        <v>440</v>
-      </c>
-      <c r="Q126" s="1">
-        <v>3600</v>
-      </c>
-      <c r="R126" s="1">
-        <v>43.6649379999999</v>
-      </c>
-      <c r="S126" s="1">
-        <v>-79.3845034</v>
-      </c>
-    </row>
-    <row r="127" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B127" s="19" t="s">
-        <v>613</v>
-      </c>
-      <c r="C127" s="20" t="s">
-        <v>614</v>
       </c>
       <c r="D127" s="1" t="s">
         <v>79</v>
@@ -9303,13 +9409,13 @@
       <c r="G127" s="1" t="s">
         <v>440</v>
       </c>
-      <c r="H127" s="43" t="s">
-        <v>615</v>
-      </c>
-      <c r="I127" s="43" t="s">
-        <v>616</v>
-      </c>
-      <c r="J127" s="43">
+      <c r="H127" s="42" t="s">
+        <v>612</v>
+      </c>
+      <c r="I127" s="42" t="s">
+        <v>613</v>
+      </c>
+      <c r="J127" s="42">
         <v>300</v>
       </c>
       <c r="K127" s="1">
@@ -9318,82 +9424,81 @@
       <c r="L127" s="1">
         <v>-79.3845034</v>
       </c>
-      <c r="M127" s="43" t="s">
-        <v>78</v>
-      </c>
-      <c r="N127" s="43"/>
-      <c r="O127" s="43">
-        <v>9097</v>
-      </c>
-      <c r="P127" s="43" t="s">
-        <v>598</v>
+      <c r="M127" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="O127" s="1">
+        <v>4037</v>
+      </c>
+      <c r="P127" s="1" t="s">
+        <v>405</v>
       </c>
       <c r="Q127" s="1">
         <v>3600</v>
       </c>
-      <c r="R127" s="43">
-        <v>43.6649689999999</v>
-      </c>
-      <c r="S127" s="43">
-        <v>-79.393966199999895</v>
-      </c>
-    </row>
-    <row r="128" spans="2:19" hidden="1" x14ac:dyDescent="0.2">
+      <c r="R127" s="1">
+        <v>43.666195299999899</v>
+      </c>
+      <c r="S127" s="1">
+        <v>-79.378280599999897</v>
+      </c>
+    </row>
+    <row r="128" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="B128" s="19" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="C128" s="20" t="s">
-        <v>602</v>
+        <v>608</v>
       </c>
       <c r="D128" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F128" s="1">
+        <v>4037</v>
+      </c>
+      <c r="G128" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="H128" s="42" t="s">
+        <v>615</v>
+      </c>
+      <c r="I128" s="42" t="s">
+        <v>616</v>
+      </c>
+      <c r="J128" s="1">
+        <v>300</v>
+      </c>
+      <c r="K128" s="1">
+        <v>43.666195299999899</v>
+      </c>
+      <c r="L128" s="1">
+        <v>-79.378280599999897</v>
+      </c>
+      <c r="M128" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="F128" s="1">
+      <c r="O128" s="1">
         <v>5329</v>
       </c>
-      <c r="G128" s="1" t="s">
+      <c r="P128" s="1" t="s">
         <v>440</v>
       </c>
-      <c r="H128" s="43" t="s">
-        <v>618</v>
-      </c>
-      <c r="I128" s="43" t="s">
-        <v>619</v>
-      </c>
-      <c r="J128" s="43">
-        <v>300</v>
-      </c>
-      <c r="K128" s="1">
+      <c r="Q128" s="1">
+        <v>3600</v>
+      </c>
+      <c r="R128" s="1">
         <v>43.6649379999999</v>
       </c>
-      <c r="L128" s="1">
+      <c r="S128" s="1">
         <v>-79.3845034</v>
-      </c>
-      <c r="M128" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="O128" s="1">
-        <v>4037</v>
-      </c>
-      <c r="P128" s="1" t="s">
-        <v>405</v>
-      </c>
-      <c r="Q128" s="1">
-        <v>3600</v>
-      </c>
-      <c r="R128" s="1">
-        <v>43.666195299999899</v>
-      </c>
-      <c r="S128" s="1">
-        <v>-79.378280599999897</v>
       </c>
     </row>
     <row r="129" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="B129" s="19" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="C129" s="20" t="s">
-        <v>614</v>
+        <v>598</v>
       </c>
       <c r="D129" s="1" t="s">
         <v>77</v>
@@ -9404,11 +9509,11 @@
       <c r="G129" s="1" t="s">
         <v>405</v>
       </c>
-      <c r="H129" s="43" t="s">
-        <v>621</v>
-      </c>
-      <c r="I129" s="43" t="s">
-        <v>622</v>
+      <c r="H129" s="42" t="s">
+        <v>615</v>
+      </c>
+      <c r="I129" s="42" t="s">
+        <v>618</v>
       </c>
       <c r="J129" s="1">
         <v>300</v>
@@ -9420,760 +9525,1155 @@
         <v>-79.378280599999897</v>
       </c>
       <c r="M129" s="1" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="O129" s="1">
-        <v>5329</v>
+        <v>5123</v>
       </c>
       <c r="P129" s="1" t="s">
-        <v>440</v>
+        <v>421</v>
       </c>
       <c r="Q129" s="1">
         <v>3600</v>
       </c>
       <c r="R129" s="1">
-        <v>43.6649379999999</v>
+        <v>43.668166499999899</v>
       </c>
       <c r="S129" s="1">
-        <v>-79.3845034</v>
+        <v>-79.369504500000005</v>
       </c>
     </row>
     <row r="130" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="B130" s="19" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="C130" s="20" t="s">
-        <v>602</v>
+        <v>608</v>
       </c>
       <c r="D130" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F130" s="1">
+        <v>5123</v>
+      </c>
+      <c r="G130" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="H130" s="42" t="s">
+        <v>612</v>
+      </c>
+      <c r="I130" s="42" t="s">
+        <v>633</v>
+      </c>
+      <c r="J130" s="1">
+        <v>300</v>
+      </c>
+      <c r="K130" s="1">
+        <v>43.668166499999899</v>
+      </c>
+      <c r="L130" s="1">
+        <v>-79.369504500000005</v>
+      </c>
+      <c r="M130" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F130" s="1">
+      <c r="O130" s="1">
         <v>4037</v>
       </c>
-      <c r="G130" s="1" t="s">
+      <c r="P130" s="1" t="s">
         <v>405</v>
       </c>
-      <c r="H130" s="43" t="s">
-        <v>621</v>
-      </c>
-      <c r="I130" s="43" t="s">
-        <v>624</v>
-      </c>
-      <c r="J130" s="1">
-        <v>300</v>
-      </c>
-      <c r="K130" s="1">
+      <c r="Q130" s="1">
+        <v>3600</v>
+      </c>
+      <c r="R130" s="1">
         <v>43.666195299999899</v>
       </c>
-      <c r="L130" s="1">
+      <c r="S130" s="1">
         <v>-79.378280599999897</v>
-      </c>
-      <c r="M130" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="O130" s="1">
-        <v>5123</v>
-      </c>
-      <c r="P130" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="Q130" s="1">
-        <v>3600</v>
-      </c>
-      <c r="R130" s="1">
-        <v>43.668166499999899</v>
-      </c>
-      <c r="S130" s="1">
-        <v>-79.369504500000005</v>
       </c>
     </row>
     <row r="131" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="B131" s="19" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="C131" s="20" t="s">
-        <v>614</v>
+        <v>541</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>86</v>
+        <v>59</v>
       </c>
       <c r="F131" s="1">
-        <v>5123</v>
+        <v>5272</v>
       </c>
       <c r="G131" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="H131" s="43" t="s">
-        <v>618</v>
-      </c>
-      <c r="I131" s="43" t="s">
-        <v>639</v>
+        <v>532</v>
+      </c>
+      <c r="H131" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="I131" s="1" t="s">
+        <v>623</v>
       </c>
       <c r="J131" s="1">
         <v>300</v>
       </c>
       <c r="K131" s="1">
-        <v>43.668166499999899</v>
+        <v>43.654397400000001</v>
       </c>
       <c r="L131" s="1">
-        <v>-79.369504500000005</v>
+        <v>-79.422612200000003</v>
       </c>
       <c r="M131" s="1" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="O131" s="1">
-        <v>4037</v>
+        <v>5266</v>
       </c>
       <c r="P131" s="1" t="s">
-        <v>405</v>
+        <v>417</v>
       </c>
       <c r="Q131" s="1">
         <v>3600</v>
       </c>
       <c r="R131" s="1">
-        <v>43.666195299999899</v>
+        <v>43.649413799999898</v>
       </c>
       <c r="S131" s="1">
-        <v>-79.378280599999897</v>
+        <v>-79.420862700000001</v>
       </c>
     </row>
     <row r="132" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
       <c r="B132" s="19" t="s">
-        <v>630</v>
+        <v>625</v>
       </c>
       <c r="C132" s="20" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="D132" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F132" s="1">
+        <v>5266</v>
+      </c>
+      <c r="G132" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="H132" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="I132" s="1" t="s">
+        <v>627</v>
+      </c>
+      <c r="J132" s="1">
+        <v>300</v>
+      </c>
+      <c r="K132" s="1">
+        <v>43.649413799999898</v>
+      </c>
+      <c r="L132" s="1">
+        <v>-79.420862700000001</v>
+      </c>
+      <c r="M132" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F132" s="1">
+      <c r="O132" s="1">
         <v>5272</v>
       </c>
-      <c r="G132" s="1" t="s">
+      <c r="P132" s="1" t="s">
         <v>532</v>
       </c>
-      <c r="H132" s="1" t="s">
-        <v>628</v>
-      </c>
-      <c r="I132" s="1" t="s">
-        <v>629</v>
-      </c>
-      <c r="J132" s="1">
-        <v>300</v>
-      </c>
-      <c r="K132" s="1">
+      <c r="Q132" s="1">
+        <v>3600</v>
+      </c>
+      <c r="R132" s="1">
         <v>43.654397400000001</v>
       </c>
-      <c r="L132" s="1">
+      <c r="S132" s="1">
         <v>-79.422612200000003</v>
       </c>
-      <c r="M132" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="O132" s="1">
-        <v>5266</v>
-      </c>
-      <c r="P132" s="1" t="s">
-        <v>417</v>
-      </c>
-      <c r="Q132" s="1">
-        <v>3600</v>
-      </c>
-      <c r="R132" s="1">
-        <v>43.649413799999898</v>
-      </c>
-      <c r="S132" s="1">
-        <v>-79.420862700000001</v>
-      </c>
-    </row>
-    <row r="133" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B133" s="19" t="s">
-        <v>631</v>
-      </c>
-      <c r="C133" s="20" t="s">
-        <v>537</v>
-      </c>
-      <c r="D133" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F133" s="1">
-        <v>5266</v>
-      </c>
-      <c r="G133" s="1" t="s">
-        <v>417</v>
-      </c>
-      <c r="H133" s="1" t="s">
-        <v>632</v>
-      </c>
-      <c r="I133" s="1" t="s">
-        <v>633</v>
-      </c>
-      <c r="J133" s="1">
-        <v>300</v>
-      </c>
-      <c r="K133" s="1">
-        <v>43.649413799999898</v>
-      </c>
-      <c r="L133" s="1">
-        <v>-79.420862700000001</v>
-      </c>
-      <c r="M133" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="O133" s="1">
-        <v>5272</v>
-      </c>
-      <c r="P133" s="1" t="s">
-        <v>532</v>
-      </c>
-      <c r="Q133" s="1">
-        <v>3600</v>
-      </c>
-      <c r="R133" s="1">
-        <v>43.654397400000001</v>
-      </c>
-      <c r="S133" s="1">
-        <v>-79.422612200000003</v>
-      </c>
-    </row>
-    <row r="134" spans="1:33" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A134" s="51" t="s">
-        <v>652</v>
-      </c>
-      <c r="B134" s="52" t="s">
+    </row>
+    <row r="133" spans="1:33" s="50" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A133" s="50" t="s">
+        <v>646</v>
+      </c>
+      <c r="B133" s="51" t="s">
+        <v>665</v>
+      </c>
+      <c r="C133" s="52" t="s">
+        <v>146</v>
+      </c>
+      <c r="D133" s="50" t="s">
+        <v>657</v>
+      </c>
+      <c r="F133" s="50">
+        <v>5819</v>
+      </c>
+      <c r="G133" s="50" t="s">
+        <v>670</v>
+      </c>
+      <c r="H133" s="50" t="s">
+        <v>666</v>
+      </c>
+      <c r="I133" s="50" t="s">
+        <v>667</v>
+      </c>
+      <c r="J133" s="50">
+        <v>300</v>
+      </c>
+      <c r="K133" s="50">
+        <v>43.653686999999998</v>
+      </c>
+      <c r="L133" s="50">
+        <v>-79.465096000000003</v>
+      </c>
+      <c r="M133" s="50" t="s">
+        <v>138</v>
+      </c>
+      <c r="O133" s="50">
+        <v>9096</v>
+      </c>
+      <c r="P133" s="50" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q133" s="50">
+        <v>3600</v>
+      </c>
+      <c r="R133" s="50">
+        <v>43.659861999999997</v>
+      </c>
+      <c r="S133" s="50">
+        <v>-79.435443899999996</v>
+      </c>
+      <c r="AG133" s="50" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="134" spans="1:33" s="50" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A134" s="50" t="s">
+        <v>646</v>
+      </c>
+      <c r="B134" s="51" t="s">
+        <v>671</v>
+      </c>
+      <c r="C134" s="52" t="s">
+        <v>287</v>
+      </c>
+      <c r="D134" s="50" t="s">
+        <v>138</v>
+      </c>
+      <c r="F134" s="50">
+        <v>9096</v>
+      </c>
+      <c r="G134" s="50" t="s">
+        <v>150</v>
+      </c>
+      <c r="H134" s="50" t="s">
+        <v>668</v>
+      </c>
+      <c r="I134" s="50" t="s">
+        <v>669</v>
+      </c>
+      <c r="J134" s="50">
+        <v>300</v>
+      </c>
+      <c r="K134" s="50">
+        <v>43.659861999999997</v>
+      </c>
+      <c r="L134" s="50">
+        <v>-79.435443899999996</v>
+      </c>
+      <c r="M134" s="50" t="s">
+        <v>657</v>
+      </c>
+      <c r="O134" s="50">
+        <v>5819</v>
+      </c>
+      <c r="P134" s="50" t="s">
+        <v>670</v>
+      </c>
+      <c r="Q134" s="50">
+        <v>3600</v>
+      </c>
+      <c r="R134" s="50">
+        <v>43.653686999999998</v>
+      </c>
+      <c r="S134" s="50">
+        <v>-79.465096000000003</v>
+      </c>
+      <c r="AG134" s="50" t="s">
         <v>673</v>
       </c>
-      <c r="C134" s="53" t="s">
-        <v>146</v>
-      </c>
-      <c r="D134" s="51" t="s">
-        <v>665</v>
-      </c>
-      <c r="F134" s="51">
-        <v>5819</v>
-      </c>
-      <c r="G134" s="51" t="s">
+    </row>
+    <row r="135" spans="1:33" s="42" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A135" s="47" t="s">
+        <v>647</v>
+      </c>
+      <c r="B135" s="48" t="s">
+        <v>674</v>
+      </c>
+      <c r="C135" s="49" t="s">
+        <v>517</v>
+      </c>
+      <c r="D135" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="E135" s="47"/>
+      <c r="F135" s="47">
+        <v>9039</v>
+      </c>
+      <c r="G135" s="47" t="s">
+        <v>518</v>
+      </c>
+      <c r="H135" s="47" t="s">
+        <v>677</v>
+      </c>
+      <c r="I135" s="47" t="s">
         <v>678</v>
       </c>
-      <c r="H134" s="51" t="s">
-        <v>674</v>
-      </c>
-      <c r="I134" s="51" t="s">
+      <c r="J135" s="47">
+        <v>300</v>
+      </c>
+      <c r="K135" s="47">
+        <v>43.6495409999999</v>
+      </c>
+      <c r="L135" s="47">
+        <v>-79.431478999999896</v>
+      </c>
+      <c r="M135" s="47" t="s">
+        <v>138</v>
+      </c>
+      <c r="N135" s="47"/>
+      <c r="O135" s="47">
+        <v>9096</v>
+      </c>
+      <c r="P135" s="47" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q135" s="47">
+        <v>3600</v>
+      </c>
+      <c r="R135" s="47">
+        <v>43.659861999999997</v>
+      </c>
+      <c r="S135" s="47">
+        <v>-79.435443899999996</v>
+      </c>
+      <c r="T135" s="47"/>
+      <c r="U135" s="47"/>
+      <c r="V135" s="47"/>
+      <c r="W135" s="47"/>
+      <c r="X135" s="47"/>
+      <c r="Y135" s="47"/>
+      <c r="Z135" s="47"/>
+      <c r="AA135" s="47"/>
+      <c r="AB135" s="47"/>
+      <c r="AC135" s="47"/>
+      <c r="AD135" s="47"/>
+      <c r="AE135" s="47"/>
+      <c r="AF135" s="47"/>
+      <c r="AG135" s="47" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="136" spans="1:33" s="42" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A136" s="47" t="s">
+        <v>647</v>
+      </c>
+      <c r="B136" s="48" t="s">
         <v>675</v>
       </c>
-      <c r="J134" s="51">
-        <v>300</v>
-      </c>
-      <c r="K134" s="51">
-        <v>43.653686999999998</v>
-      </c>
-      <c r="L134" s="51">
-        <v>-79.465096000000003</v>
-      </c>
-      <c r="M134" s="51" t="s">
+      <c r="C136" s="49" t="s">
+        <v>521</v>
+      </c>
+      <c r="D136" s="47" t="s">
         <v>138</v>
       </c>
-      <c r="O134" s="51">
+      <c r="E136" s="47"/>
+      <c r="F136" s="47">
         <v>9096</v>
       </c>
-      <c r="P134" s="51" t="s">
+      <c r="G136" s="47" t="s">
         <v>150</v>
       </c>
-      <c r="Q134" s="51">
-        <v>3600</v>
-      </c>
-      <c r="R134" s="51">
+      <c r="H136" s="47" t="s">
+        <v>676</v>
+      </c>
+      <c r="I136" s="47" t="s">
+        <v>679</v>
+      </c>
+      <c r="J136" s="47">
+        <v>300</v>
+      </c>
+      <c r="K136" s="47">
         <v>43.659861999999997</v>
       </c>
-      <c r="S134" s="51">
+      <c r="L136" s="47">
         <v>-79.435443899999996</v>
       </c>
-      <c r="AG134" s="51" t="s">
-        <v>680</v>
-      </c>
-    </row>
-    <row r="135" spans="1:33" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A135" s="51" t="s">
-        <v>652</v>
-      </c>
-      <c r="B135" s="52" t="s">
-        <v>679</v>
-      </c>
-      <c r="C135" s="53" t="s">
-        <v>287</v>
-      </c>
-      <c r="D135" s="51" t="s">
-        <v>138</v>
-      </c>
-      <c r="F135" s="51">
-        <v>9096</v>
-      </c>
-      <c r="G135" s="51" t="s">
-        <v>150</v>
-      </c>
-      <c r="H135" s="51" t="s">
-        <v>676</v>
-      </c>
-      <c r="I135" s="51" t="s">
-        <v>677</v>
-      </c>
-      <c r="J135" s="51">
-        <v>300</v>
-      </c>
-      <c r="K135" s="51">
-        <v>43.659861999999997</v>
-      </c>
-      <c r="L135" s="51">
-        <v>-79.435443899999996</v>
-      </c>
-      <c r="M135" s="51" t="s">
-        <v>665</v>
-      </c>
-      <c r="O135" s="51">
-        <v>5819</v>
-      </c>
-      <c r="P135" s="51" t="s">
-        <v>678</v>
-      </c>
-      <c r="Q135" s="51">
-        <v>3600</v>
-      </c>
-      <c r="R135" s="51">
-        <v>43.653686999999998</v>
-      </c>
-      <c r="S135" s="51">
-        <v>-79.465096000000003</v>
-      </c>
-      <c r="AG135" s="51" t="s">
+      <c r="M136" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="N136" s="47"/>
+      <c r="O136" s="47">
+        <v>9039</v>
+      </c>
+      <c r="P136" s="47" t="s">
+        <v>518</v>
+      </c>
+      <c r="Q136" s="47">
+        <v>3600</v>
+      </c>
+      <c r="R136" s="47">
+        <v>43.6495409999999</v>
+      </c>
+      <c r="S136" s="47">
+        <v>-79.431478999999896</v>
+      </c>
+      <c r="T136" s="47"/>
+      <c r="U136" s="47"/>
+      <c r="V136" s="47"/>
+      <c r="W136" s="47"/>
+      <c r="X136" s="47"/>
+      <c r="Y136" s="47"/>
+      <c r="Z136" s="47"/>
+      <c r="AA136" s="47"/>
+      <c r="AB136" s="47"/>
+      <c r="AC136" s="47"/>
+      <c r="AD136" s="47"/>
+      <c r="AE136" s="47"/>
+      <c r="AF136" s="47"/>
+      <c r="AG136" s="47" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="137" spans="1:33" s="46" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A137" s="46" t="s">
+        <v>636</v>
+      </c>
+      <c r="B137" s="53" t="s">
+        <v>639</v>
+      </c>
+      <c r="C137" s="54" t="s">
+        <v>510</v>
+      </c>
+      <c r="D137" s="46" t="s">
+        <v>49</v>
+      </c>
+      <c r="F137" s="46">
+        <v>9021</v>
+      </c>
+      <c r="G137" s="46" t="s">
+        <v>640</v>
+      </c>
+      <c r="H137" s="46" t="s">
+        <v>641</v>
+      </c>
+      <c r="I137" s="46" t="s">
+        <v>642</v>
+      </c>
+      <c r="J137" s="46">
+        <v>300</v>
+      </c>
+      <c r="K137" s="46">
+        <v>43.638885000000002</v>
+      </c>
+      <c r="L137" s="46">
+        <v>-79.446359999999899</v>
+      </c>
+      <c r="M137" s="46" t="s">
+        <v>139</v>
+      </c>
+      <c r="O137" s="46">
+        <v>5268</v>
+      </c>
+      <c r="P137" s="46" t="s">
+        <v>147</v>
+      </c>
+      <c r="Q137" s="46">
+        <v>3600</v>
+      </c>
+      <c r="R137" s="46">
+        <v>43.656353600000003</v>
+      </c>
+      <c r="S137" s="46">
+        <v>-79.452438400000005</v>
+      </c>
+      <c r="AG137" s="46" t="s">
         <v>681</v>
       </c>
     </row>
-    <row r="136" spans="1:33" s="43" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A136" s="48" t="s">
-        <v>653</v>
-      </c>
-      <c r="B136" s="49" t="s">
+    <row r="138" spans="1:33" s="46" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A138" s="46" t="s">
+        <v>636</v>
+      </c>
+      <c r="B138" s="53" t="s">
+        <v>643</v>
+      </c>
+      <c r="C138" s="54" t="s">
+        <v>512</v>
+      </c>
+      <c r="D138" s="46" t="s">
+        <v>139</v>
+      </c>
+      <c r="F138" s="46">
+        <v>5268</v>
+      </c>
+      <c r="G138" s="46" t="s">
+        <v>147</v>
+      </c>
+      <c r="H138" s="46" t="s">
+        <v>644</v>
+      </c>
+      <c r="I138" s="46" t="s">
+        <v>645</v>
+      </c>
+      <c r="J138" s="46">
+        <v>300</v>
+      </c>
+      <c r="K138" s="46">
+        <v>43.656353600000003</v>
+      </c>
+      <c r="L138" s="46">
+        <v>-79.452438400000005</v>
+      </c>
+      <c r="M138" s="46" t="s">
+        <v>49</v>
+      </c>
+      <c r="O138" s="46">
+        <v>9021</v>
+      </c>
+      <c r="P138" s="46" t="s">
+        <v>640</v>
+      </c>
+      <c r="Q138" s="46">
+        <v>3600</v>
+      </c>
+      <c r="R138" s="46">
+        <v>43.638885000000002</v>
+      </c>
+      <c r="S138" s="46">
+        <v>-79.446359999999899</v>
+      </c>
+      <c r="AG138" s="46" t="s">
         <v>682</v>
-      </c>
-      <c r="C136" s="50" t="s">
-        <v>517</v>
-      </c>
-      <c r="D136" s="48" t="s">
-        <v>35</v>
-      </c>
-      <c r="E136" s="48"/>
-      <c r="F136" s="48">
-        <v>9039</v>
-      </c>
-      <c r="G136" s="48" t="s">
-        <v>518</v>
-      </c>
-      <c r="H136" s="48" t="s">
-        <v>685</v>
-      </c>
-      <c r="I136" s="48" t="s">
-        <v>686</v>
-      </c>
-      <c r="J136" s="48">
-        <v>300</v>
-      </c>
-      <c r="K136" s="48">
-        <v>43.6495409999999</v>
-      </c>
-      <c r="L136" s="48">
-        <v>-79.431478999999896</v>
-      </c>
-      <c r="M136" s="48" t="s">
-        <v>138</v>
-      </c>
-      <c r="N136" s="48"/>
-      <c r="O136" s="48">
-        <v>9096</v>
-      </c>
-      <c r="P136" s="48" t="s">
-        <v>150</v>
-      </c>
-      <c r="Q136" s="48">
-        <v>3600</v>
-      </c>
-      <c r="R136" s="48">
-        <v>43.659861999999997</v>
-      </c>
-      <c r="S136" s="48">
-        <v>-79.435443899999996</v>
-      </c>
-      <c r="T136" s="48"/>
-      <c r="U136" s="48"/>
-      <c r="V136" s="48"/>
-      <c r="W136" s="48"/>
-      <c r="X136" s="48"/>
-      <c r="Y136" s="48"/>
-      <c r="Z136" s="48"/>
-      <c r="AA136" s="48"/>
-      <c r="AB136" s="48"/>
-      <c r="AC136" s="48"/>
-      <c r="AD136" s="48"/>
-      <c r="AE136" s="48"/>
-      <c r="AF136" s="48"/>
-      <c r="AG136" s="48" t="s">
-        <v>691</v>
-      </c>
-    </row>
-    <row r="137" spans="1:33" s="43" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A137" s="48" t="s">
-        <v>653</v>
-      </c>
-      <c r="B137" s="49" t="s">
-        <v>683</v>
-      </c>
-      <c r="C137" s="50" t="s">
-        <v>521</v>
-      </c>
-      <c r="D137" s="48" t="s">
-        <v>138</v>
-      </c>
-      <c r="E137" s="48"/>
-      <c r="F137" s="48">
-        <v>9096</v>
-      </c>
-      <c r="G137" s="48" t="s">
-        <v>150</v>
-      </c>
-      <c r="H137" s="48" t="s">
-        <v>684</v>
-      </c>
-      <c r="I137" s="48" t="s">
-        <v>687</v>
-      </c>
-      <c r="J137" s="48">
-        <v>300</v>
-      </c>
-      <c r="K137" s="48">
-        <v>43.659861999999997</v>
-      </c>
-      <c r="L137" s="48">
-        <v>-79.435443899999996</v>
-      </c>
-      <c r="M137" s="48" t="s">
-        <v>35</v>
-      </c>
-      <c r="N137" s="48"/>
-      <c r="O137" s="48">
-        <v>9039</v>
-      </c>
-      <c r="P137" s="48" t="s">
-        <v>518</v>
-      </c>
-      <c r="Q137" s="48">
-        <v>3600</v>
-      </c>
-      <c r="R137" s="48">
-        <v>43.6495409999999</v>
-      </c>
-      <c r="S137" s="48">
-        <v>-79.431478999999896</v>
-      </c>
-      <c r="T137" s="48"/>
-      <c r="U137" s="48"/>
-      <c r="V137" s="48"/>
-      <c r="W137" s="48"/>
-      <c r="X137" s="48"/>
-      <c r="Y137" s="48"/>
-      <c r="Z137" s="48"/>
-      <c r="AA137" s="48"/>
-      <c r="AB137" s="48"/>
-      <c r="AC137" s="48"/>
-      <c r="AD137" s="48"/>
-      <c r="AE137" s="48"/>
-      <c r="AF137" s="48"/>
-      <c r="AG137" s="48" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="138" spans="1:33" s="47" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A138" s="47" t="s">
-        <v>642</v>
-      </c>
-      <c r="B138" s="54" t="s">
-        <v>645</v>
-      </c>
-      <c r="C138" s="55" t="s">
-        <v>510</v>
-      </c>
-      <c r="D138" s="47" t="s">
-        <v>49</v>
-      </c>
-      <c r="F138" s="47">
-        <v>9021</v>
-      </c>
-      <c r="G138" s="47" t="s">
-        <v>646</v>
-      </c>
-      <c r="H138" s="47" t="s">
-        <v>647</v>
-      </c>
-      <c r="I138" s="47" t="s">
-        <v>648</v>
-      </c>
-      <c r="J138" s="47">
-        <v>300</v>
-      </c>
-      <c r="K138" s="47">
-        <v>43.638885000000002</v>
-      </c>
-      <c r="L138" s="47">
-        <v>-79.446359999999899</v>
-      </c>
-      <c r="M138" s="47" t="s">
-        <v>139</v>
-      </c>
-      <c r="O138" s="47">
-        <v>5268</v>
-      </c>
-      <c r="P138" s="47" t="s">
-        <v>147</v>
-      </c>
-      <c r="Q138" s="47">
-        <v>3600</v>
-      </c>
-      <c r="R138" s="47">
-        <v>43.656353600000003</v>
-      </c>
-      <c r="S138" s="47">
-        <v>-79.452438400000005</v>
-      </c>
-      <c r="AG138" s="47" t="s">
-        <v>689</v>
       </c>
     </row>
     <row r="139" spans="1:33" s="47" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A139" s="47" t="s">
-        <v>642</v>
-      </c>
-      <c r="B139" s="54" t="s">
+        <v>636</v>
+      </c>
+      <c r="B139" s="48" t="s">
+        <v>648</v>
+      </c>
+      <c r="C139" s="49" t="s">
         <v>649</v>
       </c>
-      <c r="C139" s="55" t="s">
-        <v>512</v>
-      </c>
       <c r="D139" s="47" t="s">
-        <v>139</v>
+        <v>41</v>
       </c>
       <c r="F139" s="47">
-        <v>5268</v>
+        <v>9038</v>
       </c>
       <c r="G139" s="47" t="s">
-        <v>147</v>
+        <v>650</v>
       </c>
       <c r="H139" s="47" t="s">
+        <v>651</v>
+      </c>
+      <c r="I139" s="47" t="s">
+        <v>652</v>
+      </c>
+      <c r="J139" s="47">
+        <v>300</v>
+      </c>
+      <c r="K139" s="47">
+        <v>43.654710000000001</v>
+      </c>
+      <c r="L139" s="47">
+        <v>-79.388576999999898</v>
+      </c>
+      <c r="M139" s="47" t="s">
+        <v>135</v>
+      </c>
+      <c r="O139" s="47">
+        <v>5330</v>
+      </c>
+      <c r="P139" s="47" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q139" s="47">
+        <v>3600</v>
+      </c>
+      <c r="R139" s="47">
+        <v>43.668709800000002</v>
+      </c>
+      <c r="S139" s="47">
+        <v>-79.394137900000004</v>
+      </c>
+      <c r="AG139" s="47" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="140" spans="1:33" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A140" s="47" t="s">
+        <v>636</v>
+      </c>
+      <c r="B140" s="48" t="s">
+        <v>697</v>
+      </c>
+      <c r="C140" s="49" t="s">
+        <v>701</v>
+      </c>
+      <c r="D140" s="47" t="s">
+        <v>135</v>
+      </c>
+      <c r="F140" s="47">
+        <v>5330</v>
+      </c>
+      <c r="G140" s="47" t="s">
+        <v>166</v>
+      </c>
+      <c r="H140" s="47" t="s">
+        <v>653</v>
+      </c>
+      <c r="I140" s="47" t="s">
+        <v>654</v>
+      </c>
+      <c r="J140" s="47">
+        <v>300</v>
+      </c>
+      <c r="K140" s="47">
+        <v>43.668709800000002</v>
+      </c>
+      <c r="L140" s="47">
+        <v>-79.394137900000004</v>
+      </c>
+      <c r="M140" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="O140" s="47">
+        <v>9038</v>
+      </c>
+      <c r="P140" s="47" t="s">
         <v>650</v>
       </c>
-      <c r="I139" s="47" t="s">
-        <v>651</v>
-      </c>
-      <c r="J139" s="47">
-        <v>300</v>
-      </c>
-      <c r="K139" s="47">
-        <v>43.656353600000003</v>
-      </c>
-      <c r="L139" s="47">
-        <v>-79.452438400000005</v>
-      </c>
-      <c r="M139" s="47" t="s">
-        <v>49</v>
-      </c>
-      <c r="O139" s="47">
-        <v>9021</v>
-      </c>
-      <c r="P139" s="47" t="s">
+      <c r="Q140" s="47">
+        <v>3600</v>
+      </c>
+      <c r="R140" s="47">
+        <v>43.654710000000001</v>
+      </c>
+      <c r="S140" s="47">
+        <v>-79.388576999999898</v>
+      </c>
+      <c r="AG140" s="47" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="141" spans="1:33" s="50" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A141" s="50" t="s">
         <v>646</v>
       </c>
-      <c r="Q139" s="47">
-        <v>3600</v>
-      </c>
-      <c r="R139" s="47">
-        <v>43.638885000000002</v>
-      </c>
-      <c r="S139" s="47">
-        <v>-79.446359999999899</v>
-      </c>
-      <c r="AG139" s="47" t="s">
+      <c r="B141" s="51" t="s">
+        <v>684</v>
+      </c>
+      <c r="C141" s="52" t="s">
+        <v>287</v>
+      </c>
+      <c r="D141" s="50" t="s">
+        <v>136</v>
+      </c>
+      <c r="F141" s="50">
+        <v>9092</v>
+      </c>
+      <c r="G141" s="50" t="s">
+        <v>558</v>
+      </c>
+      <c r="H141" s="50" t="s">
+        <v>687</v>
+      </c>
+      <c r="I141" s="50" t="s">
+        <v>685</v>
+      </c>
+      <c r="J141" s="50">
+        <v>300</v>
+      </c>
+      <c r="K141" s="50">
+        <v>43.665108699999898</v>
+      </c>
+      <c r="L141" s="50">
+        <v>-79.411196700000005</v>
+      </c>
+      <c r="M141" s="50" t="s">
+        <v>138</v>
+      </c>
+      <c r="O141" s="50">
+        <v>9096</v>
+      </c>
+      <c r="P141" s="50" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q141" s="50">
+        <v>3600</v>
+      </c>
+      <c r="R141" s="50">
+        <v>43.659861999999997</v>
+      </c>
+      <c r="S141" s="50">
+        <v>-79.435443899999996</v>
+      </c>
+      <c r="AG141" s="50" t="s">
         <v>690</v>
       </c>
     </row>
-    <row r="140" spans="1:33" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A140" s="51" t="s">
-        <v>642</v>
-      </c>
-      <c r="B140" s="52" t="s">
-        <v>654</v>
-      </c>
-      <c r="C140" s="53" t="s">
-        <v>655</v>
-      </c>
-      <c r="D140" s="51" t="s">
+    <row r="142" spans="1:33" s="50" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A142" s="50" t="s">
+        <v>646</v>
+      </c>
+      <c r="B142" s="51" t="s">
+        <v>686</v>
+      </c>
+      <c r="C142" s="52" t="s">
+        <v>146</v>
+      </c>
+      <c r="D142" s="50" t="s">
+        <v>138</v>
+      </c>
+      <c r="F142" s="50">
+        <v>9096</v>
+      </c>
+      <c r="G142" s="50" t="s">
+        <v>150</v>
+      </c>
+      <c r="H142" s="50" t="s">
+        <v>688</v>
+      </c>
+      <c r="I142" s="50" t="s">
+        <v>689</v>
+      </c>
+      <c r="J142" s="50">
+        <v>300</v>
+      </c>
+      <c r="K142" s="50">
+        <v>43.659861999999997</v>
+      </c>
+      <c r="L142" s="50">
+        <v>-79.435443899999996</v>
+      </c>
+      <c r="M142" s="50" t="s">
+        <v>136</v>
+      </c>
+      <c r="O142" s="50">
+        <v>9092</v>
+      </c>
+      <c r="P142" s="50" t="s">
+        <v>558</v>
+      </c>
+      <c r="Q142" s="50">
+        <v>3600</v>
+      </c>
+      <c r="R142" s="50">
+        <v>43.665108699999898</v>
+      </c>
+      <c r="S142" s="50">
+        <v>-79.411196700000005</v>
+      </c>
+      <c r="AG142" s="50" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="143" spans="1:33" s="50" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A143" s="50" t="s">
+        <v>646</v>
+      </c>
+      <c r="B143" s="51" t="s">
+        <v>691</v>
+      </c>
+      <c r="C143" s="52" t="s">
+        <v>146</v>
+      </c>
+      <c r="D143" s="50" t="s">
+        <v>136</v>
+      </c>
+      <c r="F143" s="50">
+        <v>9092</v>
+      </c>
+      <c r="G143" s="50" t="s">
+        <v>558</v>
+      </c>
+      <c r="H143" s="50" t="s">
+        <v>692</v>
+      </c>
+      <c r="I143" s="50" t="s">
+        <v>693</v>
+      </c>
+      <c r="J143" s="50">
+        <v>300</v>
+      </c>
+      <c r="K143" s="50">
+        <v>43.665108699999898</v>
+      </c>
+      <c r="L143" s="50">
+        <v>-79.411196700000005</v>
+      </c>
+      <c r="M143" s="50" t="s">
+        <v>135</v>
+      </c>
+      <c r="O143" s="50">
+        <v>5330</v>
+      </c>
+      <c r="P143" s="50" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q143" s="50">
+        <v>3600</v>
+      </c>
+      <c r="R143" s="50">
+        <v>43.668709800000002</v>
+      </c>
+      <c r="S143" s="50">
+        <v>-79.394137900000004</v>
+      </c>
+      <c r="AG143" s="50" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="144" spans="1:33" s="50" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A144" s="50" t="s">
+        <v>646</v>
+      </c>
+      <c r="B144" s="51" t="s">
+        <v>696</v>
+      </c>
+      <c r="C144" s="52" t="s">
+        <v>287</v>
+      </c>
+      <c r="D144" s="50" t="s">
+        <v>135</v>
+      </c>
+      <c r="F144" s="50">
+        <v>5330</v>
+      </c>
+      <c r="G144" s="50" t="s">
+        <v>166</v>
+      </c>
+      <c r="H144" s="50" t="s">
+        <v>694</v>
+      </c>
+      <c r="I144" s="50" t="s">
+        <v>695</v>
+      </c>
+      <c r="J144" s="50">
+        <v>300</v>
+      </c>
+      <c r="K144" s="50">
+        <v>43.668709800000002</v>
+      </c>
+      <c r="L144" s="50">
+        <v>-79.394137900000004</v>
+      </c>
+      <c r="M144" s="50" t="s">
+        <v>136</v>
+      </c>
+      <c r="O144" s="50">
+        <v>9092</v>
+      </c>
+      <c r="P144" s="50" t="s">
+        <v>558</v>
+      </c>
+      <c r="Q144" s="50">
+        <v>3600</v>
+      </c>
+      <c r="R144" s="50">
+        <v>43.665108699999898</v>
+      </c>
+      <c r="S144" s="50">
+        <v>-79.411196700000005</v>
+      </c>
+    </row>
+    <row r="145" spans="1:33" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A145" s="47" t="s">
+        <v>647</v>
+      </c>
+      <c r="B145" s="48" t="s">
+        <v>717</v>
+      </c>
+      <c r="C145" s="49" t="s">
+        <v>701</v>
+      </c>
+      <c r="D145" s="47" t="s">
+        <v>84</v>
+      </c>
+      <c r="F145" s="47">
+        <v>5612</v>
+      </c>
+      <c r="G145" s="47" t="s">
+        <v>586</v>
+      </c>
+      <c r="H145" s="47" t="s">
+        <v>718</v>
+      </c>
+      <c r="I145" s="47" t="s">
+        <v>719</v>
+      </c>
+      <c r="J145" s="47">
+        <v>300</v>
+      </c>
+      <c r="K145" s="47">
+        <v>43.6649689999999</v>
+      </c>
+      <c r="L145" s="47">
+        <v>-79.393966199999895</v>
+      </c>
+      <c r="M145" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="F140" s="51">
+      <c r="O145" s="47">
         <v>9038</v>
       </c>
-      <c r="G140" s="51" t="s">
-        <v>658</v>
-      </c>
-      <c r="H140" s="51" t="s">
-        <v>659</v>
-      </c>
-      <c r="I140" s="51" t="s">
-        <v>660</v>
-      </c>
-      <c r="J140" s="51">
-        <v>300</v>
-      </c>
-      <c r="K140" s="51">
+      <c r="P145" s="47" t="s">
+        <v>650</v>
+      </c>
+      <c r="Q145" s="47">
+        <v>3600</v>
+      </c>
+      <c r="R145" s="47">
         <v>43.654710000000001</v>
       </c>
-      <c r="L140" s="51">
+      <c r="S145" s="47">
         <v>-79.388576999999898</v>
       </c>
-      <c r="M140" s="51" t="s">
-        <v>135</v>
-      </c>
-      <c r="O140" s="51">
-        <v>5330</v>
-      </c>
-      <c r="P140" s="51" t="s">
-        <v>166</v>
-      </c>
-      <c r="Q140" s="51">
-        <v>3600</v>
-      </c>
-      <c r="R140" s="51">
-        <v>43.668709800000002</v>
-      </c>
-      <c r="S140" s="51">
-        <v>-79.394137900000004</v>
-      </c>
-      <c r="AG140" s="51" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="141" spans="1:33" s="51" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A141" s="51" t="s">
-        <v>642</v>
-      </c>
-      <c r="B141" s="52" t="s">
-        <v>656</v>
-      </c>
-      <c r="C141" s="53" t="s">
-        <v>657</v>
-      </c>
-      <c r="D141" s="51" t="s">
-        <v>135</v>
-      </c>
-      <c r="F141" s="51">
-        <v>5330</v>
-      </c>
-      <c r="G141" s="51" t="s">
-        <v>166</v>
-      </c>
-      <c r="H141" s="51" t="s">
-        <v>661</v>
-      </c>
-      <c r="I141" s="51" t="s">
-        <v>662</v>
-      </c>
-      <c r="J141" s="51">
-        <v>300</v>
-      </c>
-      <c r="K141" s="51">
-        <v>43.668709800000002</v>
-      </c>
-      <c r="L141" s="51">
-        <v>-79.394137900000004</v>
-      </c>
-      <c r="M141" s="51" t="s">
+    </row>
+    <row r="146" spans="1:33" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A146" s="47" t="s">
+        <v>647</v>
+      </c>
+      <c r="B146" s="48" t="s">
+        <v>705</v>
+      </c>
+      <c r="C146" s="49" t="s">
+        <v>552</v>
+      </c>
+      <c r="D146" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="F146" s="47">
+        <v>9090</v>
+      </c>
+      <c r="G146" s="47" t="s">
+        <v>550</v>
+      </c>
+      <c r="H146" s="47" t="s">
+        <v>706</v>
+      </c>
+      <c r="I146" s="47" t="s">
+        <v>707</v>
+      </c>
+      <c r="J146" s="47">
+        <v>300</v>
+      </c>
+      <c r="K146" s="47">
+        <v>43.661569499999899</v>
+      </c>
+      <c r="L146" s="47">
+        <v>-79.4097376</v>
+      </c>
+      <c r="M146" s="47" t="s">
+        <v>708</v>
+      </c>
+      <c r="O146" s="47">
+        <v>9036</v>
+      </c>
+      <c r="P146" s="47" t="s">
+        <v>709</v>
+      </c>
+      <c r="Q146" s="47">
+        <v>3600</v>
+      </c>
+      <c r="R146" s="47">
+        <v>43.647148000000001</v>
+      </c>
+      <c r="S146" s="47">
+        <v>-79.404032999999899</v>
+      </c>
+      <c r="AG146" s="47" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="147" spans="1:33" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A147" s="47" t="s">
+        <v>647</v>
+      </c>
+      <c r="B147" s="48" t="s">
+        <v>710</v>
+      </c>
+      <c r="C147" s="49" t="s">
+        <v>544</v>
+      </c>
+      <c r="D147" s="47" t="s">
+        <v>708</v>
+      </c>
+      <c r="F147" s="47">
+        <v>9036</v>
+      </c>
+      <c r="G147" s="47" t="s">
+        <v>709</v>
+      </c>
+      <c r="H147" s="47" t="s">
+        <v>711</v>
+      </c>
+      <c r="I147" s="47" t="s">
+        <v>712</v>
+      </c>
+      <c r="J147" s="47">
+        <v>300</v>
+      </c>
+      <c r="K147" s="47">
+        <v>43.647148000000001</v>
+      </c>
+      <c r="L147" s="47">
+        <v>-79.404032999999899</v>
+      </c>
+      <c r="M147" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="O147" s="47">
+        <v>9090</v>
+      </c>
+      <c r="P147" s="47" t="s">
+        <v>550</v>
+      </c>
+      <c r="Q147" s="47">
+        <v>3600</v>
+      </c>
+      <c r="R147" s="47">
+        <v>43.661569499999899</v>
+      </c>
+      <c r="S147" s="47">
+        <v>-79.4097376</v>
+      </c>
+      <c r="AG147" s="47" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="148" spans="1:33" s="47" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A148" s="47" t="s">
+        <v>647</v>
+      </c>
+      <c r="B148" s="47" t="s">
+        <v>715</v>
+      </c>
+      <c r="C148" s="47" t="s">
+        <v>649</v>
+      </c>
+      <c r="D148" s="47" t="s">
         <v>41</v>
       </c>
-      <c r="O141" s="51">
+      <c r="F148" s="47">
         <v>9038</v>
       </c>
-      <c r="P141" s="51" t="s">
-        <v>658</v>
-      </c>
-      <c r="Q141" s="51">
-        <v>3600</v>
-      </c>
-      <c r="R141" s="51">
+      <c r="G148" s="47" t="s">
+        <v>650</v>
+      </c>
+      <c r="H148" s="47" t="s">
+        <v>714</v>
+      </c>
+      <c r="I148" s="47" t="s">
+        <v>716</v>
+      </c>
+      <c r="J148" s="47">
+        <v>300</v>
+      </c>
+      <c r="K148" s="47">
         <v>43.654710000000001</v>
       </c>
-      <c r="S141" s="51">
+      <c r="L148" s="47">
         <v>-79.388576999999898</v>
       </c>
-      <c r="AG141" s="51" t="s">
-        <v>663</v>
-      </c>
-    </row>
-    <row r="142" spans="1:33" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B142" s="19"/>
-      <c r="C142" s="20"/>
-      <c r="F142" s="1"/>
-      <c r="O142" s="1"/>
-    </row>
-    <row r="143" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="B143" s="19"/>
-      <c r="C143" s="20"/>
-      <c r="F143" s="1"/>
-      <c r="O143" s="1"/>
-    </row>
-    <row r="144" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="B144" s="19"/>
-      <c r="C144" s="20"/>
-      <c r="F144" s="1"/>
-      <c r="O144" s="1"/>
-    </row>
-    <row r="145" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B145" s="19"/>
-      <c r="C145" s="20"/>
-      <c r="F145" s="1"/>
-      <c r="O145" s="1"/>
-    </row>
-    <row r="146" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B146" s="19"/>
-      <c r="C146" s="20"/>
-      <c r="F146" s="1"/>
-      <c r="O146" s="1"/>
-    </row>
-    <row r="147" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B147" s="19"/>
-      <c r="C147" s="20"/>
-      <c r="F147" s="1"/>
-      <c r="O147" s="1"/>
-    </row>
-    <row r="148" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B148" s="19"/>
-      <c r="C148" s="20"/>
-      <c r="F148" s="1"/>
-      <c r="O148" s="1"/>
-      <c r="AG148" s="43"/>
-    </row>
-    <row r="149" spans="2:33" x14ac:dyDescent="0.2">
-      <c r="B149" s="19"/>
-      <c r="C149" s="20"/>
-      <c r="F149" s="1"/>
-      <c r="O149" s="1"/>
+      <c r="M148" s="47" t="s">
+        <v>78</v>
+      </c>
+      <c r="O148" s="47">
+        <v>9097</v>
+      </c>
+      <c r="P148" s="47" t="s">
+        <v>594</v>
+      </c>
+      <c r="Q148" s="47">
+        <v>3600</v>
+      </c>
+      <c r="R148" s="47">
+        <v>43.6649689999999</v>
+      </c>
+      <c r="S148" s="47">
+        <v>-79.393966199999895</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:AF142" xr:uid="{00000000-0009-0000-0000-000000000000}">
+  <autoFilter ref="A2:AF148" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="0">
       <customFilters>
         <customFilter operator="notEqual" val=" "/>
       </customFilters>
     </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A100:AF139">
-      <sortCondition ref="A2:A139"/>
+    <filterColumn colId="1">
+      <filters>
+        <filter val="DT3_Bathurst-NB_College-to-Harbord"/>
+        <filter val="DT3_Bathurst-NB_Harbord-to-Bloor"/>
+        <filter val="DT3_Bathurst-NB_Queen-to-Harbord"/>
+        <filter val="DT3_Bathurst-SB_Bloor-to-Harbord"/>
+        <filter val="DT3_Bathurst-SB_Harbord-to-College"/>
+        <filter val="DT3_Bathurst-SB_Harbord-to-Queen"/>
+        <filter val="DT3_Bloor-EB_Bathurst-to-Avenue"/>
+        <filter val="DT3_Bloor-EB_Dufferin-to-Bathurst"/>
+        <filter val="DT3_Bloor-EB_Highpark-to-Dufferin"/>
+        <filter val="DT3_Bloor-EB_Runnymede-to-Highpark"/>
+        <filter val="DT3_Bloor-WB_Avenue-to-Bathurst"/>
+        <filter val="DT3_Bloor-WB_Bathurst-to-Dufferin"/>
+        <filter val="DT3_Bloor-WB_Dufferin-to-Highpark"/>
+        <filter val="DT3_Bloor-WB_Highpark-to-Runnymede"/>
+        <filter val="DT3_College-EB_Dufferin-to-Ossington"/>
+        <filter val="DT3_College-WB_Ossington-to-Dufferin"/>
+        <filter val="DT3_Dufferin-NB_College-to-Bloor"/>
+        <filter val="DT3_Dufferin-NB_Dundas-to-Bloor"/>
+        <filter val="DT3_Dufferin-NB_Dundas-to-College"/>
+        <filter val="DT3_Dufferin-SB_Bloor-to-College"/>
+        <filter val="DT3_Dufferin-SB_Bloor-to-Dundas"/>
+        <filter val="DT3_Dufferin-SB_College-to-Dundas"/>
+        <filter val="DT3_Harbord-EB_Bathurst-to-Spadina"/>
+        <filter val="DT3_Harbord-EB_Spadina-to-Queens"/>
+        <filter val="DT3_Harbord-WB_Queens-to-Spadina"/>
+        <filter val="DT3_Harbord-WB_Spadina-to-Bathurst"/>
+        <filter val="DT3_Ossington-NB_College-to-Bloor"/>
+        <filter val="DT3_Ossington-NB_Dundas-to-College"/>
+        <filter val="DT3_Ossington-SB_Bloor-to-College"/>
+        <filter val="DT3_Ossington-SB_College-to-Dundas"/>
+        <filter val="DT3_Queens-NB_College-to-Wellesley"/>
+        <filter val="DT3_Queenspark-NB_Wellesley-to-Bloor"/>
+        <filter val="DT3_Queenspark-SB_Bloor-to-Dundas"/>
+        <filter val="DT3_Queenspark-SB_Bloor-to-Hoskin"/>
+        <filter val="DT3_Queenspark-SB_Hoskin-to-Dundas"/>
+        <filter val="DT3_Queens-SB_Hoskin-to-College"/>
+        <filter val="DT3_Roncesvalles-NB_Dundas-to-Bloor"/>
+        <filter val="DT3_Roncesvalles-NB_Queen-to-Bloor"/>
+        <filter val="DT3_Roncesvalles-SB_Bloor-to-Queen"/>
+        <filter val="DT3_Spadina-NB_College-to-Harbord"/>
+        <filter val="DT3_Spadina-NB_Harbord-to-Bloor"/>
+        <filter val="DT3_Spadina-SB_Bloor-to-Harbord"/>
+        <filter val="DT3_Spadina-SB_Harbord-to-College"/>
+        <filter val="DT3_University-NB_Dundas-to-Bloor"/>
+        <filter val="DT3_University-NB_Dundas-to-Wellesley"/>
+        <filter val="DT3_Wellesley-EB_Jarvis-to-Parliament"/>
+        <filter val="DT3_Wellesley-EB_Queens-to-Yonge"/>
+        <filter val="DT3_Wellesley-EB_Yonge-to-Jarvis"/>
+        <filter val="DT3_Wellesley-WB_Jarvis-to-Parliament"/>
+        <filter val="DT3_Wellesley-WB_Jarvis-to-Yonge"/>
+        <filter val="DT3_Wellesley-WB_Yonge-to-Queens"/>
+      </filters>
+    </filterColumn>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A100:AF138">
+      <sortCondition ref="A2:A138"/>
     </sortState>
   </autoFilter>
   <mergeCells count="6">
@@ -10210,14 +10710,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="61" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="64" t="s">
+      <c r="B2" s="62"/>
+      <c r="C2" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="65"/>
+      <c r="D2" s="64"/>
       <c r="E2" s="21" t="s">
         <v>57</v>
       </c>
@@ -11425,24 +11925,24 @@
       </c>
       <c r="K61" s="22"/>
     </row>
-    <row r="62" spans="1:11" s="44" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="45" t="s">
+    <row r="62" spans="1:11" s="43" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="44" t="s">
         <v>515</v>
       </c>
-      <c r="B62" s="45" t="s">
-        <v>640</v>
-      </c>
-      <c r="C62" s="45">
+      <c r="B62" s="44" t="s">
+        <v>634</v>
+      </c>
+      <c r="C62" s="44">
         <v>9312</v>
       </c>
-      <c r="D62" s="45"/>
-      <c r="E62" s="45">
+      <c r="D62" s="44"/>
+      <c r="E62" s="44">
         <v>43.651156999999898</v>
       </c>
-      <c r="F62" s="45">
+      <c r="F62" s="44">
         <v>-79.476039999999898</v>
       </c>
-      <c r="K62" s="46"/>
+      <c r="K62" s="45"/>
     </row>
     <row r="63" spans="1:11" ht="15" x14ac:dyDescent="0.25">
       <c r="K63" s="22"/>

</xml_diff>